<commit_message>
Completed the (Not in ARS) and Skipped controls
Signed-off-by: karikarshivani <karikarshivani@gmail.com>
</commit_message>
<xml_diff>
--- a/cms-ars-3.1-high-microsoft-windows-server-2019-stig-overlay.xlsx
+++ b/cms-ars-3.1-high-microsoft-windows-server-2019-stig-overlay.xlsx
@@ -5,15 +5,14 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shivanik\Desktop\InSpec\Windows\Windows Server 2019\Overlay\High\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shivanik\Desktop\InSpec\Windows\Windows Server 2019\Overlay\High\cms-ars-3.1-high-microsoft-windows-server-2019-stig-overlay\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="27840" windowHeight="3840" tabRatio="220"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="27840" windowHeight="3840" tabRatio="220"/>
   </bookViews>
   <sheets>
     <sheet name="cmsars3.1high_w2019overlay" sheetId="1" r:id="rId1"/>
-    <sheet name="Notes" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'cmsars3.1high_w2019overlay'!$A$1:$U$304</definedName>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4427" uniqueCount="2950">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4424" uniqueCount="2947">
   <si>
     <t>refs</t>
   </si>
@@ -7737,9 +7736,6 @@
     </r>
   </si>
   <si>
-    <t>static inputs file requirement was removed by using the profile tag in inspec.yml</t>
-  </si>
-  <si>
     <t>2016 fix</t>
   </si>
   <si>
@@ -7748,9 +7744,6 @@
   <si>
     <t xml:space="preserve">(not in ARS) Add to Overlay: desc, 'caveat', 'Not applicable for this CMS ARS 3.1 overlay, since the CCEB is not applicable to CMS"
 </t>
-  </si>
-  <si>
-    <t>controls in the overlay can be broken down using 'include V-'</t>
   </si>
   <si>
     <t>2019 fix</t>
@@ -7760,9 +7753,6 @@
 New-Localuser -Name "test" -AccountExpires (Get-Date).AddDays(30)
 temporary_account_expiration = 30
 temporary_account_expiration_metadata = "30 days"</t>
-  </si>
-  <si>
-    <t>TEST: Try with 2 overlay controls and run it to see if it works</t>
   </si>
   <si>
     <t>(not in ARS)
@@ -11182,58 +11172,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>: DoD Root CA 2 DoD Root CA 3 DoD Root CA 4 DoD Root CA 5 The InstallRoot tool is available on IASE at http://iase.disa.mil/pki-pke/Pages/tools.aspx.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">This is applicable to unclassified systems. It is NA for others.
-Verify that the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <strike/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>DoD</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> CMS</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Interoperability Root Certificate Authority (CA) cross-certificates is installed in the Untrusted Certificates Store on unclassified systems.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <strike/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Open \"PowerShell\" as an administrator. Execute the following command: Get-ChildItem -Path Cert:Localmachine\\disallowed | Where {$_.Issuer -Like \"*DoD Interoperability*\" -and $_.Subject -Like \"*DoD*\"} | FL Subject, Issuer, Thumbprint, NotAfter If the following certificate \"Subject\", \"Issuer\", and \"Thumbprint\" information is not displayed, this is a finding. If an expired certificate (\"NotAfter\" date) is not listed in the results, this is not a finding. Subject: CN=DoD Root CA 2, OU=PKI, OU=DoD, O=U.S. Government, C=US Issuer: CN=DoD Interoperability Root CA 1, OU=PKI, OU=DoD, O=U.S. Government, C=US Thumbprint: 22BBE981F0694D246CC1472ED2B021DC8540A22F NotAfter: 9/6/2019 Subject: CN=DoD Root CA 3, OU=PKI, OU=DoD, O=U.S. Government, C=US Issuer: CN=DoD Interoperability Root CA 2, OU=PKI, OU=DoD, O=U.S. Government, C=US Thumbprint: FCE1B1E25374DD94F5935BEB86CA643D8C8D1FF4 NotAfter: 2/17/2019 Alternately, use the Certificates MMC snap-in: Run \"MMC\". Select \"File\", \"Add/Remove Snap-in\". Select \"Certificates\" and click \"Add\". Select \"Computer account\" and click \"Next\". Select \"Local computer: (the computer this console is running on)\" and click \"Finish\". Click \"OK\". Expand \"Certificates\" and navigate to \"Untrusted Certificates &gt;&gt; Certificates\". For each certificate with \"DoD Root CA...\" under \"Issued To\" and \"DoD Interoperability Root CA...\" under \"Issued By\": Right-click on the certificate and select \"Open\". Select the \"Details\" Tab. Scroll to the bottom and select \"Thumbprint\". If the certificates below are not listed or the value for the \"Thumbprint\" field is not as noted, this is a finding. If an expired certificate (\"Valid to\" date) is not listed in the results, this is not a finding. Issued To: DoD Root CA 2 Issued By: DoD Interoperability Root CA 1 Thumbprint: 22BBE981F0694D246CC1472ED2B021DC8540A22F Valid to: Friday, September 6, 2019 Issued To: DoD Root CA 3 Issued By: DoD Interoperability Root CA 2 Thumbprint: FFAD03329B9E527A43EEC66A56F9CBB5393E6E13 Valid to: Sunday, September 23, 2018 Issued To: DoD Root CA 3 Issued By: DoD Interoperability Root CA 2 Thumbprint: FCE1B1E25374DD94F5935BEB86CA643D8C8D1FF4 Valid to: Sunday, February 17, 2019"</t>
     </r>
   </si>
   <si>
@@ -12575,6 +12513,46 @@
   </si>
   <si>
     <t>V-73307</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This is applicable to unclassified systems. It is NA for others.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Verify that the CMS Interoperability Root Certificate Authority (CA) cross-certificates is installed in the Untrusted Certificates Store on unclassified systems.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Open \"PowerShell\" as an administrator. Execute the following command: Get-ChildItem -Path Cert:Localmachine\\disallowed | Where {$_.Issuer -Like \"*DoD Interoperability*\" -and $_.Subject -Like \"*DoD*\"} | FL Subject, Issuer, Thumbprint, NotAfter If the following certificate \"Subject\", \"Issuer\", and \"Thumbprint\" information is not displayed, this is a finding. If an expired certificate (\"NotAfter\" date) is not listed in the results, this is not a finding. Subject: CN=DoD Root CA 2, OU=PKI, OU=DoD, O=U.S. Government, C=US Issuer: CN=DoD Interoperability Root CA 1, OU=PKI, OU=DoD, O=U.S. Government, C=US Thumbprint: 22BBE981F0694D246CC1472ED2B021DC8540A22F NotAfter: 9/6/2019 Subject: CN=DoD Root CA 3, OU=PKI, OU=DoD, O=U.S. Government, C=US Issuer: CN=DoD Interoperability Root CA 2, OU=PKI, OU=DoD, O=U.S. Government, C=US Thumbprint: FCE1B1E25374DD94F5935BEB86CA643D8C8D1FF4 NotAfter: 2/17/2019 Alternately, use the Certificates MMC snap-in: Run \"MMC\". Select \"File\", \"Add/Remove Snap-in\". Select \"Certificates\" and click \"Add\". Select \"Computer account\" and click \"Next\". Select \"Local computer: (the computer this console is running on)\" and click \"Finish\". Click \"OK\". Expand \"Certificates\" and navigate to \"Untrusted Certificates &gt;&gt; Certificates\". For each certificate with \"DoD Root CA...\" under \"Issued To\" and \"DoD Interoperability Root CA...\" under \"Issued By\": Right-click on the certificate and select \"Open\". Select the \"Details\" Tab. Scroll to the bottom and select \"Thumbprint\". If the certificates below are not listed or the value for the \"Thumbprint\" field is not as noted, this is a finding. If an expired certificate (\"Valid to\" date) is not listed in the results, this is not a finding. Issued To: DoD Root CA 2 Issued By: DoD Interoperability Root CA 1 Thumbprint: 22BBE981F0694D246CC1472ED2B021DC8540A22F Valid to: Friday, September 6, 2019 Issued To: DoD Root CA 3 Issued By: DoD Interoperability Root CA 2 Thumbprint: FFAD03329B9E527A43EEC66A56F9CBB5393E6E13 Valid to: Sunday, September 23, 2018 Issued To: DoD Root CA 3 Issued By: DoD Interoperability Root CA 2 Thumbprint: FCE1B1E25374DD94F5935BEB86CA643D8C8D1FF4 Valid to: Sunday, February 17, 2019"</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -13488,7 +13466,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D303" sqref="D303"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.42578125" defaultRowHeight="114.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -13576,10 +13554,10 @@
         <v>2181</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>2282</v>
+        <v>2281</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>2286</v>
+        <v>2284</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -13600,10 +13578,10 @@
         <v>988</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>2399</v>
+        <v>2396</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>2291</v>
+        <v>2288</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>994</v>
@@ -13651,13 +13629,13 @@
         <v>1286</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>2400</v>
+        <v>2397</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>2401</v>
+        <v>2398</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>2292</v>
+        <v>2289</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>1292</v>
@@ -13705,13 +13683,13 @@
         <v>1941</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>2400</v>
+        <v>2397</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>2402</v>
+        <v>2399</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>2293</v>
+        <v>2290</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>1292</v>
@@ -13759,13 +13737,13 @@
         <v>411</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>2403</v>
+        <v>2400</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>2404</v>
+        <v>2401</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>2405</v>
+        <v>2402</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>417</v>
@@ -13810,13 +13788,13 @@
         <v>886</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>2406</v>
+        <v>2403</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>2407</v>
+        <v>2404</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>2408</v>
+        <v>2405</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>417</v>
@@ -13864,10 +13842,10 @@
         <v>572</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>2409</v>
+        <v>2406</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>2294</v>
+        <v>2291</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>578</v>
@@ -13918,10 +13896,10 @@
         <v>1729</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>2410</v>
+        <v>2407</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>2295</v>
+        <v>2292</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>578</v>
@@ -13966,16 +13944,16 @@
         <v>0.5</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>2385</v>
+        <v>2382</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>2411</v>
+        <v>2408</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>2412</v>
+        <v>2409</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>2413</v>
+        <v>2410</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>562</v>
@@ -14023,13 +14001,13 @@
         <v>2280</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>2414</v>
+        <v>2411</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>2415</v>
+        <v>2412</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>2416</v>
+        <v>2413</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>1435</v>
@@ -14059,13 +14037,13 @@
         <v>9</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>2384</v>
+        <v>2381</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>2371</v>
+        <v>2368</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>2287</v>
+        <v>2285</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -14083,19 +14061,19 @@
         <v>205</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>2417</v>
+        <v>2414</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>2418</v>
+        <v>2415</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>2296</v>
+        <v>2293</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>211</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>2297</v>
+        <v>2294</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>206</v>
@@ -14137,19 +14115,19 @@
         <v>241</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>2419</v>
+        <v>2416</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>2420</v>
+        <v>2417</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>2298</v>
+        <v>2295</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>211</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>2297</v>
+        <v>2294</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>206</v>
@@ -14191,19 +14169,19 @@
         <v>582</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>2421</v>
+        <v>2418</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>2422</v>
+        <v>2419</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>2299</v>
+        <v>2296</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>211</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>2297</v>
+        <v>2294</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>206</v>
@@ -14245,19 +14223,19 @@
         <v>684</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>2419</v>
+        <v>2416</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>2423</v>
+        <v>2420</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>2300</v>
+        <v>2297</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>211</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>2297</v>
+        <v>2294</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>206</v>
@@ -14291,20 +14269,20 @@
       <c r="B15" s="5" t="s">
         <v>2180</v>
       </c>
-      <c r="C15" s="2">
-        <v>0.5</v>
+      <c r="C15" s="7">
+        <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>121</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>2424</v>
+        <v>2421</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>2425</v>
+        <v>2422</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>2426</v>
+        <v>2423</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>127</v>
@@ -14347,20 +14325,20 @@
       <c r="B16" s="5" t="s">
         <v>2180</v>
       </c>
-      <c r="C16" s="2">
-        <v>0.5</v>
+      <c r="C16" s="7">
+        <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>744</v>
       </c>
       <c r="E16" s="2" t="s">
+        <v>2421</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>2424</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>2427</v>
-      </c>
       <c r="G16" s="2" t="s">
-        <v>2428</v>
+        <v>2425</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>127</v>
@@ -14403,20 +14381,20 @@
       <c r="B17" s="5" t="s">
         <v>2180</v>
       </c>
-      <c r="C17" s="2">
-        <v>0.5</v>
+      <c r="C17" s="7">
+        <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>1642</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>2424</v>
+        <v>2421</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>2429</v>
+        <v>2426</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>2430</v>
+        <v>2427</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>127</v>
@@ -14467,13 +14445,13 @@
         <v>59</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>2431</v>
+        <v>2428</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>2432</v>
+        <v>2429</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>2433</v>
+        <v>2430</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>65</v>
@@ -14518,13 +14496,13 @@
         <v>150</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>2434</v>
+        <v>2431</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>2435</v>
+        <v>2432</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>2436</v>
+        <v>2433</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>65</v>
@@ -14569,13 +14547,13 @@
         <v>184</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>2437</v>
+        <v>2434</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>2438</v>
+        <v>2435</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>2439</v>
+        <v>2436</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>65</v>
@@ -14620,13 +14598,13 @@
         <v>288</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>2440</v>
+        <v>2437</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>2441</v>
+        <v>2438</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>2301</v>
+        <v>2298</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>65</v>
@@ -14671,13 +14649,13 @@
         <v>300</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>2442</v>
+        <v>2439</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>2443</v>
+        <v>2440</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>2444</v>
+        <v>2441</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>65</v>
@@ -14722,13 +14700,13 @@
         <v>672</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>2445</v>
+        <v>2442</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>2446</v>
+        <v>2443</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>2447</v>
+        <v>2444</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>65</v>
@@ -14773,13 +14751,13 @@
         <v>838</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>2448</v>
+        <v>2445</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>2449</v>
+        <v>2446</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>2450</v>
+        <v>2447</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>65</v>
@@ -14824,13 +14802,13 @@
         <v>912</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>2451</v>
+        <v>2448</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>2452</v>
+        <v>2449</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>2453</v>
+        <v>2450</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>65</v>
@@ -14875,13 +14853,13 @@
         <v>918</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>2454</v>
+        <v>2451</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>2455</v>
+        <v>2452</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>2456</v>
+        <v>2453</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>65</v>
@@ -14926,13 +14904,13 @@
         <v>1027</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>2457</v>
+        <v>2454</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>2458</v>
+        <v>2455</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>2459</v>
+        <v>2456</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>65</v>
@@ -14980,7 +14958,7 @@
         <v>1224</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>2460</v>
+        <v>2457</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>2185</v>
@@ -15028,13 +15006,13 @@
         <v>1255</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>2461</v>
+        <v>2458</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>2462</v>
+        <v>2459</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>2463</v>
+        <v>2460</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>65</v>
@@ -15082,10 +15060,10 @@
         <v>1262</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>2464</v>
+        <v>2461</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>2302</v>
+        <v>2299</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>65</v>
@@ -15130,13 +15108,13 @@
         <v>2104</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>2465</v>
+        <v>2462</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>2466</v>
+        <v>2463</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>2467</v>
+        <v>2464</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>65</v>
@@ -15181,13 +15159,13 @@
         <v>8</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>2468</v>
+        <v>2465</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>2469</v>
+        <v>2466</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>2470</v>
+        <v>2467</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>15</v>
@@ -15232,13 +15210,13 @@
         <v>37</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>2471</v>
+        <v>2468</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>2472</v>
+        <v>2469</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>2473</v>
+        <v>2470</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>15</v>
@@ -15283,13 +15261,13 @@
         <v>92</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>2474</v>
+        <v>2471</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>2475</v>
+        <v>2472</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>2476</v>
+        <v>2473</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>15</v>
@@ -15334,13 +15312,13 @@
         <v>144</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>2477</v>
+        <v>2474</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>2478</v>
+        <v>2475</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>2479</v>
+        <v>2476</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>15</v>
@@ -15385,13 +15363,13 @@
         <v>190</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>2480</v>
+        <v>2477</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>2481</v>
+        <v>2478</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>2482</v>
+        <v>2479</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>15</v>
@@ -15436,13 +15414,13 @@
         <v>294</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>2483</v>
+        <v>2480</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>2484</v>
+        <v>2481</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>2485</v>
+        <v>2482</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>15</v>
@@ -15487,13 +15465,13 @@
         <v>333</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>2486</v>
+        <v>2483</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>2487</v>
+        <v>2484</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>2488</v>
+        <v>2485</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>15</v>
@@ -15538,13 +15516,13 @@
         <v>365</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>2489</v>
+        <v>2486</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>2490</v>
+        <v>2487</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>2303</v>
+        <v>2300</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>15</v>
@@ -15589,13 +15567,13 @@
         <v>449</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>2491</v>
+        <v>2488</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>2492</v>
+        <v>2489</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>2493</v>
+        <v>2490</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>15</v>
@@ -15640,13 +15618,13 @@
         <v>468</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>2494</v>
+        <v>2491</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>2495</v>
+        <v>2492</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>2496</v>
+        <v>2493</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>15</v>
@@ -15691,13 +15669,13 @@
         <v>565</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>2497</v>
+        <v>2494</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>2498</v>
+        <v>2495</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>2499</v>
+        <v>2496</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>15</v>
@@ -15742,13 +15720,13 @@
         <v>588</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>2483</v>
+        <v>2480</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>2500</v>
+        <v>2497</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>2304</v>
+        <v>2301</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>15</v>
@@ -15793,13 +15771,13 @@
         <v>800</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>2501</v>
+        <v>2498</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>2502</v>
+        <v>2499</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>2503</v>
+        <v>2500</v>
       </c>
       <c r="H44" s="2" t="s">
         <v>15</v>
@@ -15847,10 +15825,10 @@
         <v>874</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>2504</v>
+        <v>2501</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>2505</v>
+        <v>2502</v>
       </c>
       <c r="H45" s="2" t="s">
         <v>15</v>
@@ -15895,13 +15873,13 @@
         <v>906</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>2506</v>
+        <v>2503</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>2507</v>
+        <v>2504</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>2508</v>
+        <v>2505</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>15</v>
@@ -15946,13 +15924,13 @@
         <v>924</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>2509</v>
+        <v>2506</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>2510</v>
+        <v>2507</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>2511</v>
+        <v>2508</v>
       </c>
       <c r="H47" s="2" t="s">
         <v>15</v>
@@ -15997,13 +15975,13 @@
         <v>1008</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>2512</v>
+        <v>2509</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>2513</v>
+        <v>2510</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>2305</v>
+        <v>2302</v>
       </c>
       <c r="H48" s="2" t="s">
         <v>15</v>
@@ -16048,13 +16026,13 @@
         <v>1083</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>2514</v>
+        <v>2511</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>2515</v>
+        <v>2512</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>2306</v>
+        <v>2303</v>
       </c>
       <c r="H49" s="2" t="s">
         <v>15</v>
@@ -16099,13 +16077,13 @@
         <v>1240</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>2516</v>
+        <v>2513</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>2517</v>
+        <v>2514</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>2518</v>
+        <v>2515</v>
       </c>
       <c r="H50" s="2" t="s">
         <v>15</v>
@@ -16150,13 +16128,13 @@
         <v>1511</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>2519</v>
+        <v>2516</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>2520</v>
+        <v>2517</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>2521</v>
+        <v>2518</v>
       </c>
       <c r="H51" s="2" t="s">
         <v>15</v>
@@ -16201,13 +16179,13 @@
         <v>1551</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>2522</v>
+        <v>2519</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>2523</v>
+        <v>2520</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>2524</v>
+        <v>2521</v>
       </c>
       <c r="H52" s="2" t="s">
         <v>15</v>
@@ -16252,13 +16230,13 @@
         <v>1557</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>2525</v>
+        <v>2522</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>2526</v>
+        <v>2523</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>2307</v>
+        <v>2304</v>
       </c>
       <c r="H53" s="2" t="s">
         <v>15</v>
@@ -16303,13 +16281,13 @@
         <v>1563</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>2527</v>
+        <v>2524</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>2528</v>
+        <v>2525</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>2529</v>
+        <v>2526</v>
       </c>
       <c r="H54" s="2" t="s">
         <v>15</v>
@@ -16357,10 +16335,10 @@
         <v>1610</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>2530</v>
+        <v>2527</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>2308</v>
+        <v>2305</v>
       </c>
       <c r="H55" s="2" t="s">
         <v>15</v>
@@ -16408,10 +16386,10 @@
         <v>1670</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>2531</v>
+        <v>2528</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>2532</v>
+        <v>2529</v>
       </c>
       <c r="H56" s="2" t="s">
         <v>15</v>
@@ -16456,13 +16434,13 @@
         <v>1676</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>2533</v>
+        <v>2530</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>2534</v>
+        <v>2531</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>2535</v>
+        <v>2532</v>
       </c>
       <c r="H57" s="2" t="s">
         <v>15</v>
@@ -16507,13 +16485,13 @@
         <v>1822</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>2536</v>
+        <v>2533</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>2537</v>
+        <v>2534</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>2538</v>
+        <v>2535</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>15</v>
@@ -16558,13 +16536,13 @@
         <v>1856</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>2539</v>
+        <v>2536</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>2540</v>
+        <v>2537</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>2541</v>
+        <v>2538</v>
       </c>
       <c r="H59" s="2" t="s">
         <v>15</v>
@@ -16609,13 +16587,13 @@
         <v>2030</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>2542</v>
+        <v>2539</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>2543</v>
+        <v>2540</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>2544</v>
+        <v>2541</v>
       </c>
       <c r="H60" s="2" t="s">
         <v>15</v>
@@ -16660,13 +16638,13 @@
         <v>2057</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>2545</v>
+        <v>2542</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>2546</v>
+        <v>2543</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>2547</v>
+        <v>2544</v>
       </c>
       <c r="H61" s="2" t="s">
         <v>15</v>
@@ -16711,13 +16689,13 @@
         <v>2110</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>2548</v>
+        <v>2545</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>2549</v>
+        <v>2546</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>2550</v>
+        <v>2547</v>
       </c>
       <c r="H62" s="2" t="s">
         <v>15</v>
@@ -16762,13 +16740,13 @@
         <v>2125</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>2551</v>
+        <v>2548</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>2552</v>
+        <v>2549</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>2309</v>
+        <v>2306</v>
       </c>
       <c r="H63" s="2" t="s">
         <v>15</v>
@@ -16810,16 +16788,16 @@
         <v>0.5</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>2391</v>
+        <v>2388</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>1523</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>2553</v>
+        <v>2550</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>2392</v>
+        <v>2389</v>
       </c>
       <c r="H64" s="2" t="s">
         <v>1528</v>
@@ -16852,7 +16830,7 @@
         <v>9</v>
       </c>
       <c r="S64" s="2" t="s">
-        <v>2390</v>
+        <v>2387</v>
       </c>
     </row>
     <row r="65" spans="1:20" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -16873,10 +16851,10 @@
         <v>595</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>2554</v>
+        <v>2551</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>2310</v>
+        <v>2307</v>
       </c>
       <c r="H65" s="2" t="s">
         <v>601</v>
@@ -16918,16 +16896,16 @@
         <v>0.5</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>2388</v>
+        <v>2385</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>1628</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>2555</v>
+        <v>2552</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>2556</v>
+        <v>2553</v>
       </c>
       <c r="H66" s="2" t="s">
         <v>1634</v>
@@ -16957,10 +16935,10 @@
         <v>9</v>
       </c>
       <c r="S66" s="2" t="s">
-        <v>2387</v>
+        <v>2384</v>
       </c>
       <c r="T66" s="2" t="s">
-        <v>2389</v>
+        <v>2386</v>
       </c>
     </row>
     <row r="67" spans="1:20" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -16981,16 +16959,16 @@
         <v>1380</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>2910</v>
+        <v>2906</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>2911</v>
+        <v>2907</v>
       </c>
       <c r="H67" s="2" t="s">
         <v>2054</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>2311</v>
+        <v>2308</v>
       </c>
       <c r="J67" s="2" t="s">
         <v>1381</v>
@@ -17017,7 +16995,7 @@
         <v>9</v>
       </c>
       <c r="S67" s="2" t="s">
-        <v>2290</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="68" spans="1:20" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -17038,16 +17016,16 @@
         <v>1380</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>2912</v>
+        <v>2908</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>2913</v>
+        <v>2909</v>
       </c>
       <c r="H68" s="2" t="s">
         <v>1386</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>2283</v>
+        <v>2282</v>
       </c>
       <c r="J68" s="2" t="s">
         <v>1381</v>
@@ -17074,7 +17052,7 @@
         <v>9</v>
       </c>
       <c r="S68" s="2" t="s">
-        <v>2914</v>
+        <v>2910</v>
       </c>
     </row>
     <row r="69" spans="1:20" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -17092,13 +17070,13 @@
         <v>1344</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>2557</v>
+        <v>2554</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>2558</v>
+        <v>2555</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>2312</v>
+        <v>2309</v>
       </c>
       <c r="H69" s="2" t="s">
         <v>1350</v>
@@ -17143,13 +17121,13 @@
         <v>998</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>2559</v>
+        <v>2556</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>2560</v>
+        <v>2557</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>2313</v>
+        <v>2310</v>
       </c>
       <c r="H70" s="2" t="s">
         <v>1004</v>
@@ -17197,13 +17175,13 @@
         <v>1869</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>2559</v>
+        <v>2556</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>2561</v>
+        <v>2558</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>2314</v>
+        <v>2311</v>
       </c>
       <c r="H71" s="2" t="s">
         <v>1004</v>
@@ -17251,13 +17229,13 @@
         <v>167</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>2562</v>
+        <v>2559</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>2563</v>
+        <v>2560</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>2315</v>
+        <v>2312</v>
       </c>
       <c r="H72" s="2" t="s">
         <v>173</v>
@@ -17305,13 +17283,13 @@
         <v>385</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>2564</v>
+        <v>2561</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>2565</v>
+        <v>2562</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>2316</v>
+        <v>2313</v>
       </c>
       <c r="H73" s="2" t="s">
         <v>173</v>
@@ -17359,13 +17337,13 @@
         <v>525</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>2566</v>
+        <v>2563</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>2567</v>
+        <v>2564</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>2317</v>
+        <v>2314</v>
       </c>
       <c r="H74" s="2" t="s">
         <v>173</v>
@@ -17413,13 +17391,13 @@
         <v>625</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>2568</v>
+        <v>2565</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>2569</v>
+        <v>2566</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>2318</v>
+        <v>2315</v>
       </c>
       <c r="H75" s="2" t="s">
         <v>173</v>
@@ -17467,13 +17445,13 @@
         <v>644</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>2570</v>
+        <v>2567</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>2571</v>
+        <v>2568</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>2572</v>
+        <v>2569</v>
       </c>
       <c r="H76" s="2" t="s">
         <v>173</v>
@@ -17521,13 +17499,13 @@
         <v>710</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>2573</v>
+        <v>2570</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>2574</v>
+        <v>2571</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>2319</v>
+        <v>2316</v>
       </c>
       <c r="H77" s="2" t="s">
         <v>173</v>
@@ -17575,13 +17553,13 @@
         <v>724</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>2575</v>
+        <v>2572</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>2576</v>
+        <v>2573</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>2577</v>
+        <v>2574</v>
       </c>
       <c r="H78" s="2" t="s">
         <v>173</v>
@@ -17629,13 +17607,13 @@
         <v>860</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>2578</v>
+        <v>2575</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>2579</v>
+        <v>2576</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>2320</v>
+        <v>2317</v>
       </c>
       <c r="H79" s="2" t="s">
         <v>173</v>
@@ -17683,13 +17661,13 @@
         <v>1118</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>2580</v>
+        <v>2577</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>2581</v>
+        <v>2578</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>2321</v>
+        <v>2318</v>
       </c>
       <c r="H80" s="2" t="s">
         <v>173</v>
@@ -17737,13 +17715,13 @@
         <v>1268</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>2582</v>
+        <v>2579</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>2583</v>
+        <v>2580</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>2584</v>
+        <v>2581</v>
       </c>
       <c r="H81" s="2" t="s">
         <v>173</v>
@@ -17791,13 +17769,13 @@
         <v>1308</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>2580</v>
+        <v>2577</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>2585</v>
+        <v>2582</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>2322</v>
+        <v>2319</v>
       </c>
       <c r="H82" s="2" t="s">
         <v>173</v>
@@ -17845,13 +17823,13 @@
         <v>1389</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>2586</v>
+        <v>2583</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>2587</v>
+        <v>2584</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>2588</v>
+        <v>2585</v>
       </c>
       <c r="H83" s="2" t="s">
         <v>173</v>
@@ -17899,13 +17877,13 @@
         <v>1410</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>2589</v>
+        <v>2586</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>2590</v>
+        <v>2587</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>2323</v>
+        <v>2320</v>
       </c>
       <c r="H84" s="2" t="s">
         <v>173</v>
@@ -17953,13 +17931,13 @@
         <v>1539</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>2591</v>
+        <v>2588</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>2592</v>
+        <v>2589</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>2593</v>
+        <v>2590</v>
       </c>
       <c r="H85" s="2" t="s">
         <v>173</v>
@@ -18007,13 +17985,13 @@
         <v>1545</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>2564</v>
+        <v>2561</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>2594</v>
+        <v>2591</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>2324</v>
+        <v>2321</v>
       </c>
       <c r="H86" s="2" t="s">
         <v>173</v>
@@ -18061,13 +18039,13 @@
         <v>1591</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>2566</v>
+        <v>2563</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>2595</v>
+        <v>2592</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>2325</v>
+        <v>2322</v>
       </c>
       <c r="H87" s="2" t="s">
         <v>173</v>
@@ -18115,13 +18093,13 @@
         <v>1790</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>2596</v>
+        <v>2593</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>2597</v>
+        <v>2594</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>2326</v>
+        <v>2323</v>
       </c>
       <c r="H88" s="2" t="s">
         <v>173</v>
@@ -18169,13 +18147,13 @@
         <v>1796</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>2573</v>
+        <v>2570</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>2598</v>
+        <v>2595</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>2327</v>
+        <v>2324</v>
       </c>
       <c r="H89" s="2" t="s">
         <v>173</v>
@@ -18223,13 +18201,13 @@
         <v>1809</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>2599</v>
+        <v>2596</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>2600</v>
+        <v>2597</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>2328</v>
+        <v>2325</v>
       </c>
       <c r="H90" s="2" t="s">
         <v>173</v>
@@ -18277,13 +18255,13 @@
         <v>1905</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>2601</v>
+        <v>2598</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>2602</v>
+        <v>2599</v>
       </c>
       <c r="G91" s="2" t="s">
-        <v>2603</v>
+        <v>2600</v>
       </c>
       <c r="H91" s="2" t="s">
         <v>173</v>
@@ -18331,13 +18309,13 @@
         <v>1967</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>2604</v>
+        <v>2601</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>2605</v>
+        <v>2602</v>
       </c>
       <c r="G92" s="2" t="s">
-        <v>2329</v>
+        <v>2326</v>
       </c>
       <c r="H92" s="2" t="s">
         <v>173</v>
@@ -18385,13 +18363,13 @@
         <v>1993</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>2606</v>
+        <v>2603</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>2607</v>
+        <v>2604</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>2330</v>
+        <v>2327</v>
       </c>
       <c r="H93" s="2" t="s">
         <v>173</v>
@@ -18439,13 +18417,13 @@
         <v>2011</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>2608</v>
+        <v>2605</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>2609</v>
+        <v>2606</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>2331</v>
+        <v>2328</v>
       </c>
       <c r="H94" s="2" t="s">
         <v>173</v>
@@ -18493,13 +18471,13 @@
         <v>2043</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>2589</v>
+        <v>2586</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>2610</v>
+        <v>2607</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>2332</v>
+        <v>2329</v>
       </c>
       <c r="H95" s="2" t="s">
         <v>173</v>
@@ -18547,13 +18525,13 @@
         <v>2085</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>2606</v>
+        <v>2603</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>2611</v>
+        <v>2608</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>2333</v>
+        <v>2330</v>
       </c>
       <c r="H96" s="2" t="s">
         <v>173</v>
@@ -18601,13 +18579,13 @@
         <v>2091</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>2604</v>
+        <v>2601</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>2612</v>
+        <v>2609</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>2334</v>
+        <v>2331</v>
       </c>
       <c r="H97" s="2" t="s">
         <v>173</v>
@@ -18655,13 +18633,13 @@
         <v>650</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>2613</v>
+        <v>2610</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>2614</v>
+        <v>2611</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>2335</v>
+        <v>2332</v>
       </c>
       <c r="H98" s="2" t="s">
         <v>656</v>
@@ -18709,13 +18687,13 @@
         <v>28</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>2615</v>
+        <v>2612</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>2616</v>
+        <v>2613</v>
       </c>
       <c r="G99" s="2" t="s">
-        <v>2336</v>
+        <v>2333</v>
       </c>
       <c r="H99" s="2" t="s">
         <v>34</v>
@@ -18760,13 +18738,13 @@
         <v>43</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>2617</v>
+        <v>2614</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>2618</v>
+        <v>2615</v>
       </c>
       <c r="G100" s="2" t="s">
-        <v>2337</v>
+        <v>2334</v>
       </c>
       <c r="H100" s="2" t="s">
         <v>34</v>
@@ -18811,13 +18789,13 @@
         <v>275</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>2619</v>
+        <v>2616</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>2620</v>
+        <v>2617</v>
       </c>
       <c r="G101" s="2" t="s">
-        <v>2338</v>
+        <v>2335</v>
       </c>
       <c r="H101" s="2" t="s">
         <v>34</v>
@@ -18862,13 +18840,13 @@
         <v>339</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>2621</v>
+        <v>2618</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>2622</v>
+        <v>2619</v>
       </c>
       <c r="G102" s="2" t="s">
-        <v>2339</v>
+        <v>2336</v>
       </c>
       <c r="H102" s="2" t="s">
         <v>34</v>
@@ -18913,13 +18891,13 @@
         <v>461</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>2623</v>
+        <v>2620</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>2624</v>
+        <v>2621</v>
       </c>
       <c r="G103" s="2" t="s">
-        <v>2340</v>
+        <v>2337</v>
       </c>
       <c r="H103" s="2" t="s">
         <v>34</v>
@@ -18967,13 +18945,13 @@
         <v>660</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>2621</v>
+        <v>2618</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>2625</v>
+        <v>2622</v>
       </c>
       <c r="G104" s="2" t="s">
-        <v>2341</v>
+        <v>2338</v>
       </c>
       <c r="H104" s="2" t="s">
         <v>34</v>
@@ -19018,13 +18996,13 @@
         <v>951</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>2626</v>
+        <v>2623</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>2627</v>
+        <v>2624</v>
       </c>
       <c r="G105" s="2" t="s">
-        <v>2342</v>
+        <v>2339</v>
       </c>
       <c r="H105" s="2" t="s">
         <v>34</v>
@@ -19069,13 +19047,13 @@
         <v>1280</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>2617</v>
+        <v>2614</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>2628</v>
+        <v>2625</v>
       </c>
       <c r="G106" s="2" t="s">
-        <v>2343</v>
+        <v>2340</v>
       </c>
       <c r="H106" s="2" t="s">
         <v>34</v>
@@ -19120,13 +19098,13 @@
         <v>2079</v>
       </c>
       <c r="E107" s="2" t="s">
+        <v>2623</v>
+      </c>
+      <c r="F107" s="2" t="s">
         <v>2626</v>
       </c>
-      <c r="F107" s="2" t="s">
-        <v>2629</v>
-      </c>
       <c r="G107" s="2" t="s">
-        <v>2344</v>
+        <v>2341</v>
       </c>
       <c r="H107" s="2" t="s">
         <v>34</v>
@@ -19171,13 +19149,13 @@
         <v>50</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>2630</v>
+        <v>2627</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>2631</v>
+        <v>2628</v>
       </c>
       <c r="G108" s="2" t="s">
-        <v>2345</v>
+        <v>2342</v>
       </c>
       <c r="H108" s="2" t="s">
         <v>56</v>
@@ -19222,13 +19200,13 @@
         <v>115</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>2632</v>
+        <v>2629</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>2633</v>
+        <v>2630</v>
       </c>
       <c r="G109" s="2" t="s">
-        <v>2346</v>
+        <v>2343</v>
       </c>
       <c r="H109" s="2" t="s">
         <v>56</v>
@@ -19275,10 +19253,10 @@
         <v>392</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>2634</v>
+        <v>2631</v>
       </c>
       <c r="G110" s="2" t="s">
-        <v>2347</v>
+        <v>2344</v>
       </c>
       <c r="H110" s="2" t="s">
         <v>398</v>
@@ -19328,10 +19306,10 @@
         <v>392</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>2635</v>
+        <v>2632</v>
       </c>
       <c r="G111" s="2" t="s">
-        <v>2348</v>
+        <v>2345</v>
       </c>
       <c r="H111" s="2" t="s">
         <v>398</v>
@@ -19382,10 +19360,10 @@
         <v>509</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>2636</v>
+        <v>2633</v>
       </c>
       <c r="G112" s="2" t="s">
-        <v>2349</v>
+        <v>2346</v>
       </c>
       <c r="H112" s="2" t="s">
         <v>515</v>
@@ -19433,10 +19411,10 @@
         <v>509</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>2637</v>
+        <v>2634</v>
       </c>
       <c r="G113" s="2" t="s">
-        <v>2350</v>
+        <v>2347</v>
       </c>
       <c r="H113" s="2" t="s">
         <v>515</v>
@@ -19484,10 +19462,10 @@
         <v>509</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>2638</v>
+        <v>2635</v>
       </c>
       <c r="G114" s="2" t="s">
-        <v>2351</v>
+        <v>2348</v>
       </c>
       <c r="H114" s="2" t="s">
         <v>515</v>
@@ -19529,16 +19507,16 @@
         <v>0.3</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>2386</v>
+        <v>2383</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>2153</v>
       </c>
       <c r="F115" s="4" t="s">
-        <v>2947</v>
+        <v>2943</v>
       </c>
       <c r="G115" s="4" t="s">
-        <v>2948</v>
+        <v>2944</v>
       </c>
       <c r="H115" s="2" t="s">
         <v>2159</v>
@@ -19568,7 +19546,7 @@
         <v>9</v>
       </c>
       <c r="S115" s="11" t="s">
-        <v>2949</v>
+        <v>2945</v>
       </c>
     </row>
     <row r="116" spans="1:19" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -19586,13 +19564,13 @@
         <v>2116</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>2639</v>
+        <v>2636</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>2640</v>
+        <v>2637</v>
       </c>
       <c r="G116" s="2" t="s">
-        <v>2641</v>
+        <v>2638</v>
       </c>
       <c r="H116" s="2" t="s">
         <v>2121</v>
@@ -19643,10 +19621,10 @@
         <v>931</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>2642</v>
+        <v>2639</v>
       </c>
       <c r="G117" s="2" t="s">
-        <v>2643</v>
+        <v>2640</v>
       </c>
       <c r="H117" s="2" t="s">
         <v>937</v>
@@ -19697,10 +19675,10 @@
         <v>964</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>2644</v>
+        <v>2641</v>
       </c>
       <c r="G118" s="2" t="s">
-        <v>2645</v>
+        <v>2642</v>
       </c>
       <c r="H118" s="2" t="s">
         <v>937</v>
@@ -19751,10 +19729,10 @@
         <v>1974</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>2646</v>
+        <v>2643</v>
       </c>
       <c r="G119" s="2" t="s">
-        <v>2647</v>
+        <v>2644</v>
       </c>
       <c r="H119" s="2" t="s">
         <v>937</v>
@@ -19802,13 +19780,13 @@
         <v>401</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>2648</v>
+        <v>2645</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>2649</v>
+        <v>2646</v>
       </c>
       <c r="G120" s="2" t="s">
-        <v>2650</v>
+        <v>2647</v>
       </c>
       <c r="H120" s="2" t="s">
         <v>407</v>
@@ -19858,10 +19836,10 @@
         <v>427</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>2651</v>
+        <v>2648</v>
       </c>
       <c r="G121" s="2" t="s">
-        <v>2352</v>
+        <v>2349</v>
       </c>
       <c r="H121" s="2" t="s">
         <v>433</v>
@@ -19894,7 +19872,7 @@
         <v>2179</v>
       </c>
       <c r="S121" s="2" t="s">
-        <v>2890</v>
+        <v>2887</v>
       </c>
     </row>
     <row r="122" spans="1:19" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -19914,10 +19892,10 @@
         <v>1716</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>2652</v>
+        <v>2649</v>
       </c>
       <c r="G122" s="2" t="s">
-        <v>2353</v>
+        <v>2350</v>
       </c>
       <c r="H122" s="2" t="s">
         <v>433</v>
@@ -19950,7 +19928,7 @@
         <v>2179</v>
       </c>
       <c r="S122" s="2" t="s">
-        <v>2891</v>
+        <v>2888</v>
       </c>
     </row>
     <row r="123" spans="1:19" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -19970,10 +19948,10 @@
         <v>1231</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>2653</v>
+        <v>2650</v>
       </c>
       <c r="G123" s="2" t="s">
-        <v>2354</v>
+        <v>2351</v>
       </c>
       <c r="H123" s="2" t="s">
         <v>1237</v>
@@ -20075,7 +20053,7 @@
         <v>19</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>2654</v>
+        <v>2651</v>
       </c>
       <c r="G125" s="2" t="s">
         <v>2187</v>
@@ -20126,7 +20104,7 @@
         <v>79</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>2655</v>
+        <v>2652</v>
       </c>
       <c r="G126" s="2" t="s">
         <v>2188</v>
@@ -20177,10 +20155,10 @@
         <v>86</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>2656</v>
+        <v>2653</v>
       </c>
       <c r="G127" s="2" t="s">
-        <v>2355</v>
+        <v>2352</v>
       </c>
       <c r="H127" s="2" t="s">
         <v>25</v>
@@ -20228,10 +20206,10 @@
         <v>99</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>2657</v>
+        <v>2654</v>
       </c>
       <c r="G128" s="2" t="s">
-        <v>2658</v>
+        <v>2655</v>
       </c>
       <c r="H128" s="2" t="s">
         <v>25</v>
@@ -20279,10 +20257,10 @@
         <v>132</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>2659</v>
+        <v>2656</v>
       </c>
       <c r="G129" s="4" t="s">
-        <v>2918</v>
+        <v>2914</v>
       </c>
       <c r="H129" s="2" t="s">
         <v>25</v>
@@ -20331,10 +20309,10 @@
         <v>132</v>
       </c>
       <c r="F130" s="2" t="s">
-        <v>2660</v>
+        <v>2657</v>
       </c>
       <c r="G130" s="4" t="s">
-        <v>2919</v>
+        <v>2915</v>
       </c>
       <c r="H130" s="2" t="s">
         <v>25</v>
@@ -20383,7 +20361,7 @@
         <v>178</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>2661</v>
+        <v>2658</v>
       </c>
       <c r="G131" s="2" t="s">
         <v>2189</v>
@@ -20434,10 +20412,10 @@
         <v>132</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>2662</v>
+        <v>2659</v>
       </c>
       <c r="G132" s="4" t="s">
-        <v>2920</v>
+        <v>2916</v>
       </c>
       <c r="H132" s="2" t="s">
         <v>25</v>
@@ -20486,10 +20464,10 @@
         <v>282</v>
       </c>
       <c r="F133" s="2" t="s">
-        <v>2663</v>
+        <v>2660</v>
       </c>
       <c r="G133" s="2" t="s">
-        <v>2664</v>
+        <v>2661</v>
       </c>
       <c r="H133" s="2" t="s">
         <v>25</v>
@@ -20534,13 +20512,13 @@
         <v>345</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>2665</v>
+        <v>2662</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>2666</v>
+        <v>2663</v>
       </c>
       <c r="G134" s="2" t="s">
-        <v>2356</v>
+        <v>2353</v>
       </c>
       <c r="H134" s="2" t="s">
         <v>25</v>
@@ -20588,7 +20566,7 @@
         <v>352</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>2667</v>
+        <v>2664</v>
       </c>
       <c r="G135" s="2" t="s">
         <v>2190</v>
@@ -20639,10 +20617,10 @@
         <v>372</v>
       </c>
       <c r="F136" s="2" t="s">
-        <v>2668</v>
+        <v>2665</v>
       </c>
       <c r="G136" s="4" t="s">
-        <v>2921</v>
+        <v>2917</v>
       </c>
       <c r="H136" s="2" t="s">
         <v>25</v>
@@ -20691,10 +20669,10 @@
         <v>379</v>
       </c>
       <c r="F137" s="2" t="s">
-        <v>2669</v>
+        <v>2666</v>
       </c>
       <c r="G137" s="4" t="s">
-        <v>2946</v>
+        <v>2942</v>
       </c>
       <c r="H137" s="2" t="s">
         <v>25</v>
@@ -20743,10 +20721,10 @@
         <v>132</v>
       </c>
       <c r="F138" s="2" t="s">
-        <v>2670</v>
+        <v>2667</v>
       </c>
       <c r="G138" s="4" t="s">
-        <v>2945</v>
+        <v>2941</v>
       </c>
       <c r="H138" s="2" t="s">
         <v>25</v>
@@ -20795,10 +20773,10 @@
         <v>132</v>
       </c>
       <c r="F139" s="2" t="s">
-        <v>2671</v>
+        <v>2668</v>
       </c>
       <c r="G139" s="4" t="s">
-        <v>2944</v>
+        <v>2940</v>
       </c>
       <c r="H139" s="2" t="s">
         <v>25</v>
@@ -20847,10 +20825,10 @@
         <v>132</v>
       </c>
       <c r="F140" s="2" t="s">
-        <v>2672</v>
+        <v>2669</v>
       </c>
       <c r="G140" s="4" t="s">
-        <v>2943</v>
+        <v>2939</v>
       </c>
       <c r="H140" s="2" t="s">
         <v>25</v>
@@ -20899,7 +20877,7 @@
         <v>475</v>
       </c>
       <c r="F141" s="2" t="s">
-        <v>2673</v>
+        <v>2670</v>
       </c>
       <c r="G141" s="2" t="s">
         <v>2191</v>
@@ -20950,10 +20928,10 @@
         <v>132</v>
       </c>
       <c r="F142" s="2" t="s">
-        <v>2674</v>
+        <v>2671</v>
       </c>
       <c r="G142" s="4" t="s">
-        <v>2942</v>
+        <v>2938</v>
       </c>
       <c r="H142" s="2" t="s">
         <v>25</v>
@@ -21002,7 +20980,7 @@
         <v>488</v>
       </c>
       <c r="F143" s="2" t="s">
-        <v>2675</v>
+        <v>2672</v>
       </c>
       <c r="G143" s="2" t="s">
         <v>2192</v>
@@ -21053,10 +21031,10 @@
         <v>495</v>
       </c>
       <c r="F144" s="2" t="s">
-        <v>2676</v>
+        <v>2673</v>
       </c>
       <c r="G144" s="2" t="s">
-        <v>2677</v>
+        <v>2674</v>
       </c>
       <c r="H144" s="2" t="s">
         <v>25</v>
@@ -21104,7 +21082,7 @@
         <v>502</v>
       </c>
       <c r="F145" s="2" t="s">
-        <v>2678</v>
+        <v>2675</v>
       </c>
       <c r="G145" s="2" t="s">
         <v>2193</v>
@@ -21155,7 +21133,7 @@
         <v>519</v>
       </c>
       <c r="F146" s="2" t="s">
-        <v>2679</v>
+        <v>2676</v>
       </c>
       <c r="G146" s="2" t="s">
         <v>2194</v>
@@ -21206,7 +21184,7 @@
         <v>533</v>
       </c>
       <c r="F147" s="2" t="s">
-        <v>2680</v>
+        <v>2677</v>
       </c>
       <c r="G147" s="2" t="s">
         <v>2195</v>
@@ -21257,10 +21235,10 @@
         <v>619</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>2681</v>
+        <v>2678</v>
       </c>
       <c r="G148" s="4" t="s">
-        <v>2941</v>
+        <v>2937</v>
       </c>
       <c r="H148" s="2" t="s">
         <v>25</v>
@@ -21305,7 +21283,7 @@
         <v>691</v>
       </c>
       <c r="F149" s="2" t="s">
-        <v>2682</v>
+        <v>2679</v>
       </c>
       <c r="G149" s="2" t="s">
         <v>2196</v>
@@ -21356,10 +21334,10 @@
         <v>132</v>
       </c>
       <c r="F150" s="2" t="s">
-        <v>2683</v>
+        <v>2680</v>
       </c>
       <c r="G150" s="4" t="s">
-        <v>2940</v>
+        <v>2936</v>
       </c>
       <c r="H150" s="2" t="s">
         <v>25</v>
@@ -21408,10 +21386,10 @@
         <v>704</v>
       </c>
       <c r="F151" s="2" t="s">
-        <v>2684</v>
+        <v>2681</v>
       </c>
       <c r="G151" s="2" t="s">
-        <v>2357</v>
+        <v>2354</v>
       </c>
       <c r="H151" s="2" t="s">
         <v>25</v>
@@ -21459,7 +21437,7 @@
         <v>731</v>
       </c>
       <c r="F152" s="2" t="s">
-        <v>2685</v>
+        <v>2682</v>
       </c>
       <c r="G152" s="2" t="s">
         <v>2197</v>
@@ -21510,10 +21488,10 @@
         <v>738</v>
       </c>
       <c r="F153" s="2" t="s">
-        <v>2686</v>
+        <v>2683</v>
       </c>
       <c r="G153" s="2" t="s">
-        <v>2687</v>
+        <v>2684</v>
       </c>
       <c r="H153" s="2" t="s">
         <v>25</v>
@@ -21561,10 +21539,10 @@
         <v>757</v>
       </c>
       <c r="F154" s="2" t="s">
-        <v>2688</v>
+        <v>2685</v>
       </c>
       <c r="G154" s="2" t="s">
-        <v>2358</v>
+        <v>2355</v>
       </c>
       <c r="H154" s="2" t="s">
         <v>25</v>
@@ -21612,7 +21590,7 @@
         <v>773</v>
       </c>
       <c r="F155" s="2" t="s">
-        <v>2689</v>
+        <v>2686</v>
       </c>
       <c r="G155" s="2" t="s">
         <v>2198</v>
@@ -21663,10 +21641,10 @@
         <v>780</v>
       </c>
       <c r="F156" s="2" t="s">
-        <v>2690</v>
+        <v>2687</v>
       </c>
       <c r="G156" s="2" t="s">
-        <v>2359</v>
+        <v>2356</v>
       </c>
       <c r="H156" s="2" t="s">
         <v>25</v>
@@ -21714,10 +21692,10 @@
         <v>893</v>
       </c>
       <c r="F157" s="2" t="s">
-        <v>2691</v>
+        <v>2688</v>
       </c>
       <c r="G157" s="2" t="s">
-        <v>2360</v>
+        <v>2357</v>
       </c>
       <c r="H157" s="2" t="s">
         <v>25</v>
@@ -21761,10 +21739,10 @@
         <v>540</v>
       </c>
       <c r="F158" s="2" t="s">
-        <v>2692</v>
+        <v>2689</v>
       </c>
       <c r="G158" s="2" t="s">
-        <v>2693</v>
+        <v>2690</v>
       </c>
       <c r="H158" s="2" t="s">
         <v>25</v>
@@ -21812,10 +21790,10 @@
         <v>981</v>
       </c>
       <c r="F159" s="2" t="s">
-        <v>2694</v>
+        <v>2691</v>
       </c>
       <c r="G159" s="4" t="s">
-        <v>2939</v>
+        <v>2935</v>
       </c>
       <c r="H159" s="2" t="s">
         <v>25</v>
@@ -21864,10 +21842,10 @@
         <v>132</v>
       </c>
       <c r="F160" s="2" t="s">
-        <v>2695</v>
+        <v>2692</v>
       </c>
       <c r="G160" s="4" t="s">
-        <v>2938</v>
+        <v>2934</v>
       </c>
       <c r="H160" s="2" t="s">
         <v>25</v>
@@ -21912,7 +21890,7 @@
         <v>1050</v>
       </c>
       <c r="F161" s="2" t="s">
-        <v>2696</v>
+        <v>2693</v>
       </c>
       <c r="G161" s="2" t="s">
         <v>2199</v>
@@ -21963,10 +21941,10 @@
         <v>1067</v>
       </c>
       <c r="F162" s="2" t="s">
-        <v>2697</v>
+        <v>2694</v>
       </c>
       <c r="G162" s="2" t="s">
-        <v>2698</v>
+        <v>2695</v>
       </c>
       <c r="H162" s="2" t="s">
         <v>25</v>
@@ -22014,10 +21992,10 @@
         <v>132</v>
       </c>
       <c r="F163" s="2" t="s">
-        <v>2699</v>
+        <v>2696</v>
       </c>
       <c r="G163" s="4" t="s">
-        <v>2937</v>
+        <v>2933</v>
       </c>
       <c r="H163" s="2" t="s">
         <v>25</v>
@@ -22063,13 +22041,13 @@
         <v>1095</v>
       </c>
       <c r="E164" s="2" t="s">
-        <v>2700</v>
+        <v>2697</v>
       </c>
       <c r="F164" s="2" t="s">
-        <v>2701</v>
+        <v>2698</v>
       </c>
       <c r="G164" s="2" t="s">
-        <v>2702</v>
+        <v>2699</v>
       </c>
       <c r="H164" s="2" t="s">
         <v>25</v>
@@ -22117,10 +22095,10 @@
         <v>1125</v>
       </c>
       <c r="F165" s="2" t="s">
-        <v>2703</v>
+        <v>2700</v>
       </c>
       <c r="G165" s="2" t="s">
-        <v>2704</v>
+        <v>2701</v>
       </c>
       <c r="H165" s="2" t="s">
         <v>25</v>
@@ -22168,10 +22146,10 @@
         <v>1157</v>
       </c>
       <c r="F166" s="2" t="s">
-        <v>2705</v>
+        <v>2702</v>
       </c>
       <c r="G166" s="2" t="s">
-        <v>2361</v>
+        <v>2358</v>
       </c>
       <c r="H166" s="2" t="s">
         <v>25</v>
@@ -22219,10 +22197,10 @@
         <v>132</v>
       </c>
       <c r="F167" s="2" t="s">
-        <v>2706</v>
+        <v>2703</v>
       </c>
       <c r="G167" s="4" t="s">
-        <v>2936</v>
+        <v>2932</v>
       </c>
       <c r="H167" s="2" t="s">
         <v>25</v>
@@ -22271,10 +22249,10 @@
         <v>132</v>
       </c>
       <c r="F168" s="2" t="s">
-        <v>2707</v>
+        <v>2704</v>
       </c>
       <c r="G168" s="4" t="s">
-        <v>2935</v>
+        <v>2931</v>
       </c>
       <c r="H168" s="2" t="s">
         <v>25</v>
@@ -22323,10 +22301,10 @@
         <v>1210</v>
       </c>
       <c r="F169" s="2" t="s">
-        <v>2708</v>
+        <v>2705</v>
       </c>
       <c r="G169" s="2" t="s">
-        <v>2362</v>
+        <v>2359</v>
       </c>
       <c r="H169" s="2" t="s">
         <v>25</v>
@@ -22368,16 +22346,16 @@
         <v>0.5</v>
       </c>
       <c r="D170" s="4" t="s">
-        <v>2906</v>
+        <v>2902</v>
       </c>
       <c r="E170" s="4" t="s">
-        <v>2907</v>
+        <v>2903</v>
       </c>
       <c r="F170" s="4" t="s">
-        <v>2908</v>
+        <v>2904</v>
       </c>
       <c r="G170" s="4" t="s">
-        <v>2909</v>
+        <v>2905</v>
       </c>
       <c r="H170" s="2" t="s">
         <v>25</v>
@@ -22407,7 +22385,7 @@
         <v>9</v>
       </c>
       <c r="S170" s="2" t="s">
-        <v>2905</v>
+        <v>2901</v>
       </c>
     </row>
     <row r="171" spans="1:19" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -22428,10 +22406,10 @@
         <v>132</v>
       </c>
       <c r="F171" s="2" t="s">
-        <v>2709</v>
+        <v>2706</v>
       </c>
       <c r="G171" s="4" t="s">
-        <v>2934</v>
+        <v>2930</v>
       </c>
       <c r="H171" s="2" t="s">
         <v>25</v>
@@ -22480,10 +22458,10 @@
         <v>1338</v>
       </c>
       <c r="F172" s="2" t="s">
-        <v>2710</v>
+        <v>2707</v>
       </c>
       <c r="G172" s="2" t="s">
-        <v>2363</v>
+        <v>2360</v>
       </c>
       <c r="H172" s="2" t="s">
         <v>25</v>
@@ -22531,10 +22509,10 @@
         <v>132</v>
       </c>
       <c r="F173" s="2" t="s">
-        <v>2711</v>
+        <v>2708</v>
       </c>
       <c r="G173" s="4" t="s">
-        <v>2933</v>
+        <v>2929</v>
       </c>
       <c r="H173" s="2" t="s">
         <v>25</v>
@@ -22583,10 +22561,10 @@
         <v>132</v>
       </c>
       <c r="F174" s="2" t="s">
-        <v>2712</v>
+        <v>2709</v>
       </c>
       <c r="G174" s="4" t="s">
-        <v>2932</v>
+        <v>2928</v>
       </c>
       <c r="H174" s="2" t="s">
         <v>25</v>
@@ -22635,10 +22613,10 @@
         <v>132</v>
       </c>
       <c r="F175" s="2" t="s">
-        <v>2713</v>
+        <v>2710</v>
       </c>
       <c r="G175" s="4" t="s">
-        <v>2931</v>
+        <v>2927</v>
       </c>
       <c r="H175" s="2" t="s">
         <v>25</v>
@@ -22687,7 +22665,7 @@
         <v>502</v>
       </c>
       <c r="F176" s="2" t="s">
-        <v>2714</v>
+        <v>2711</v>
       </c>
       <c r="G176" s="2" t="s">
         <v>2200</v>
@@ -22738,7 +22716,7 @@
         <v>1450</v>
       </c>
       <c r="F177" s="2" t="s">
-        <v>2715</v>
+        <v>2712</v>
       </c>
       <c r="G177" s="2" t="s">
         <v>2201</v>
@@ -22789,7 +22767,7 @@
         <v>1457</v>
       </c>
       <c r="F178" s="2" t="s">
-        <v>2716</v>
+        <v>2713</v>
       </c>
       <c r="G178" s="2" t="s">
         <v>2202</v>
@@ -22840,10 +22818,10 @@
         <v>1471</v>
       </c>
       <c r="F179" s="2" t="s">
-        <v>2717</v>
+        <v>2714</v>
       </c>
       <c r="G179" s="2" t="s">
-        <v>2718</v>
+        <v>2715</v>
       </c>
       <c r="H179" s="2" t="s">
         <v>25</v>
@@ -22887,7 +22865,7 @@
         <v>540</v>
       </c>
       <c r="F180" s="2" t="s">
-        <v>2719</v>
+        <v>2716</v>
       </c>
       <c r="G180" s="2" t="s">
         <v>2203</v>
@@ -22938,10 +22916,10 @@
         <v>1484</v>
       </c>
       <c r="F181" s="2" t="s">
-        <v>2720</v>
+        <v>2717</v>
       </c>
       <c r="G181" s="2" t="s">
-        <v>2364</v>
+        <v>2361</v>
       </c>
       <c r="H181" s="2" t="s">
         <v>25</v>
@@ -22989,10 +22967,10 @@
         <v>132</v>
       </c>
       <c r="F182" s="2" t="s">
-        <v>2721</v>
+        <v>2718</v>
       </c>
       <c r="G182" s="4" t="s">
-        <v>2930</v>
+        <v>2926</v>
       </c>
       <c r="H182" s="2" t="s">
         <v>25</v>
@@ -23041,10 +23019,10 @@
         <v>132</v>
       </c>
       <c r="F183" s="2" t="s">
-        <v>2722</v>
+        <v>2719</v>
       </c>
       <c r="G183" s="4" t="s">
-        <v>2929</v>
+        <v>2925</v>
       </c>
       <c r="H183" s="2" t="s">
         <v>25</v>
@@ -23093,10 +23071,10 @@
         <v>1533</v>
       </c>
       <c r="F184" s="2" t="s">
-        <v>2723</v>
+        <v>2720</v>
       </c>
       <c r="G184" s="2" t="s">
-        <v>2724</v>
+        <v>2721</v>
       </c>
       <c r="H184" s="2" t="s">
         <v>25</v>
@@ -23144,10 +23122,10 @@
         <v>1570</v>
       </c>
       <c r="F185" s="2" t="s">
-        <v>2725</v>
+        <v>2722</v>
       </c>
       <c r="G185" s="2" t="s">
-        <v>2726</v>
+        <v>2723</v>
       </c>
       <c r="H185" s="2" t="s">
         <v>25</v>
@@ -23195,10 +23173,10 @@
         <v>132</v>
       </c>
       <c r="F186" s="2" t="s">
-        <v>2727</v>
+        <v>2724</v>
       </c>
       <c r="G186" s="4" t="s">
-        <v>2928</v>
+        <v>2924</v>
       </c>
       <c r="H186" s="2" t="s">
         <v>25</v>
@@ -23244,13 +23222,13 @@
         <v>1622</v>
       </c>
       <c r="E187" s="2" t="s">
-        <v>2728</v>
+        <v>2725</v>
       </c>
       <c r="F187" s="2" t="s">
-        <v>2729</v>
+        <v>2726</v>
       </c>
       <c r="G187" s="2" t="s">
-        <v>2730</v>
+        <v>2727</v>
       </c>
       <c r="H187" s="2" t="s">
         <v>25</v>
@@ -23298,7 +23276,7 @@
         <v>1662</v>
       </c>
       <c r="F188" s="2" t="s">
-        <v>2731</v>
+        <v>2728</v>
       </c>
       <c r="G188" s="2" t="s">
         <v>2204</v>
@@ -23349,7 +23327,7 @@
         <v>1690</v>
       </c>
       <c r="F189" s="2" t="s">
-        <v>2732</v>
+        <v>2729</v>
       </c>
       <c r="G189" s="2" t="s">
         <v>2205</v>
@@ -23400,10 +23378,10 @@
         <v>132</v>
       </c>
       <c r="F190" s="2" t="s">
-        <v>2733</v>
+        <v>2730</v>
       </c>
       <c r="G190" s="4" t="s">
-        <v>2927</v>
+        <v>2923</v>
       </c>
       <c r="H190" s="2" t="s">
         <v>25</v>
@@ -23452,10 +23430,10 @@
         <v>1771</v>
       </c>
       <c r="F191" s="2" t="s">
-        <v>2734</v>
+        <v>2731</v>
       </c>
       <c r="G191" s="2" t="s">
-        <v>2365</v>
+        <v>2362</v>
       </c>
       <c r="H191" s="2" t="s">
         <v>25</v>
@@ -23503,10 +23481,10 @@
         <v>132</v>
       </c>
       <c r="F192" s="2" t="s">
-        <v>2735</v>
+        <v>2732</v>
       </c>
       <c r="G192" s="4" t="s">
-        <v>2926</v>
+        <v>2922</v>
       </c>
       <c r="H192" s="2" t="s">
         <v>25</v>
@@ -23555,7 +23533,7 @@
         <v>1784</v>
       </c>
       <c r="F193" s="2" t="s">
-        <v>2736</v>
+        <v>2733</v>
       </c>
       <c r="G193" s="2" t="s">
         <v>2206</v>
@@ -23606,7 +23584,7 @@
         <v>1829</v>
       </c>
       <c r="F194" s="2" t="s">
-        <v>2737</v>
+        <v>2734</v>
       </c>
       <c r="G194" s="2" t="s">
         <v>2207</v>
@@ -23657,7 +23635,7 @@
         <v>1850</v>
       </c>
       <c r="F195" s="2" t="s">
-        <v>2738</v>
+        <v>2735</v>
       </c>
       <c r="G195" s="2" t="s">
         <v>2208</v>
@@ -23708,10 +23686,10 @@
         <v>1863</v>
       </c>
       <c r="F196" s="2" t="s">
-        <v>2739</v>
+        <v>2736</v>
       </c>
       <c r="G196" s="2" t="s">
-        <v>2740</v>
+        <v>2737</v>
       </c>
       <c r="H196" s="2" t="s">
         <v>25</v>
@@ -23759,10 +23737,10 @@
         <v>1876</v>
       </c>
       <c r="F197" s="2" t="s">
-        <v>2741</v>
+        <v>2738</v>
       </c>
       <c r="G197" s="2" t="s">
-        <v>2742</v>
+        <v>2739</v>
       </c>
       <c r="H197" s="2" t="s">
         <v>25</v>
@@ -23810,10 +23788,10 @@
         <v>1893</v>
       </c>
       <c r="F198" s="2" t="s">
-        <v>2743</v>
+        <v>2740</v>
       </c>
       <c r="G198" s="2" t="s">
-        <v>2744</v>
+        <v>2741</v>
       </c>
       <c r="H198" s="2" t="s">
         <v>25</v>
@@ -23861,10 +23839,10 @@
         <v>1919</v>
       </c>
       <c r="F199" s="2" t="s">
-        <v>2745</v>
+        <v>2742</v>
       </c>
       <c r="G199" s="2" t="s">
-        <v>2746</v>
+        <v>2743</v>
       </c>
       <c r="H199" s="2" t="s">
         <v>25</v>
@@ -23912,10 +23890,10 @@
         <v>1926</v>
       </c>
       <c r="F200" s="2" t="s">
-        <v>2747</v>
+        <v>2744</v>
       </c>
       <c r="G200" s="2" t="s">
-        <v>2748</v>
+        <v>2745</v>
       </c>
       <c r="H200" s="2" t="s">
         <v>25</v>
@@ -23963,10 +23941,10 @@
         <v>132</v>
       </c>
       <c r="F201" s="2" t="s">
-        <v>2749</v>
+        <v>2746</v>
       </c>
       <c r="G201" s="4" t="s">
-        <v>2925</v>
+        <v>2921</v>
       </c>
       <c r="H201" s="2" t="s">
         <v>25</v>
@@ -24015,10 +23993,10 @@
         <v>132</v>
       </c>
       <c r="F202" s="2" t="s">
-        <v>2750</v>
+        <v>2747</v>
       </c>
       <c r="G202" s="4" t="s">
-        <v>2924</v>
+        <v>2920</v>
       </c>
       <c r="H202" s="2" t="s">
         <v>25</v>
@@ -24067,10 +24045,10 @@
         <v>1987</v>
       </c>
       <c r="F203" s="2" t="s">
-        <v>2751</v>
+        <v>2748</v>
       </c>
       <c r="G203" s="2" t="s">
-        <v>2366</v>
+        <v>2363</v>
       </c>
       <c r="H203" s="2" t="s">
         <v>25</v>
@@ -24112,16 +24090,16 @@
         <v>0.5</v>
       </c>
       <c r="D204" s="4" t="s">
-        <v>2370</v>
+        <v>2367</v>
       </c>
       <c r="E204" s="2" t="s">
         <v>1999</v>
       </c>
       <c r="F204" s="4" t="s">
-        <v>2752</v>
+        <v>2749</v>
       </c>
       <c r="G204" s="4" t="s">
-        <v>2753</v>
+        <v>2750</v>
       </c>
       <c r="H204" s="2" t="s">
         <v>25</v>
@@ -24151,10 +24129,10 @@
         <v>9</v>
       </c>
       <c r="S204" s="2" t="s">
-        <v>2369</v>
+        <v>2366</v>
       </c>
       <c r="T204" s="2" t="s">
-        <v>2373</v>
+        <v>2370</v>
       </c>
     </row>
     <row r="205" spans="1:20" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -24175,10 +24153,10 @@
         <v>132</v>
       </c>
       <c r="F205" s="2" t="s">
-        <v>2754</v>
+        <v>2751</v>
       </c>
       <c r="G205" s="4" t="s">
-        <v>2923</v>
+        <v>2919</v>
       </c>
       <c r="H205" s="2" t="s">
         <v>25</v>
@@ -24227,10 +24205,10 @@
         <v>2163</v>
       </c>
       <c r="F206" s="2" t="s">
-        <v>2755</v>
+        <v>2752</v>
       </c>
       <c r="G206" s="2" t="s">
-        <v>2367</v>
+        <v>2364</v>
       </c>
       <c r="H206" s="2" t="s">
         <v>25</v>
@@ -24278,7 +24256,7 @@
         <v>851</v>
       </c>
       <c r="F207" s="2" t="s">
-        <v>2756</v>
+        <v>2753</v>
       </c>
       <c r="G207" s="2" t="s">
         <v>2209</v>
@@ -24329,7 +24307,7 @@
         <v>1302</v>
       </c>
       <c r="F208" s="2" t="s">
-        <v>2757</v>
+        <v>2754</v>
       </c>
       <c r="G208" s="2" t="s">
         <v>2210</v>
@@ -24380,7 +24358,7 @@
         <v>1754</v>
       </c>
       <c r="F209" s="2" t="s">
-        <v>2758</v>
+        <v>2755</v>
       </c>
       <c r="G209" s="2" t="s">
         <v>2211</v>
@@ -24428,13 +24406,13 @@
         <v>1246</v>
       </c>
       <c r="E210" s="2" t="s">
-        <v>2759</v>
+        <v>2756</v>
       </c>
       <c r="F210" s="2" t="s">
-        <v>2760</v>
+        <v>2757</v>
       </c>
       <c r="G210" s="2" t="s">
-        <v>2761</v>
+        <v>2758</v>
       </c>
       <c r="H210" s="2" t="s">
         <v>1252</v>
@@ -24464,10 +24442,10 @@
         <v>9</v>
       </c>
       <c r="S210" s="12" t="s">
-        <v>2375</v>
+        <v>2372</v>
       </c>
       <c r="T210" s="2" t="s">
-        <v>2376</v>
+        <v>2373</v>
       </c>
     </row>
     <row r="211" spans="1:20" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -24488,10 +24466,10 @@
         <v>258</v>
       </c>
       <c r="F211" s="2" t="s">
-        <v>2762</v>
+        <v>2759</v>
       </c>
       <c r="G211" s="2" t="s">
-        <v>2763</v>
+        <v>2760</v>
       </c>
       <c r="H211" s="2" t="s">
         <v>264</v>
@@ -24536,10 +24514,10 @@
         <v>306</v>
       </c>
       <c r="E212" s="2" t="s">
-        <v>2764</v>
+        <v>2761</v>
       </c>
       <c r="F212" s="2" t="s">
-        <v>2765</v>
+        <v>2762</v>
       </c>
       <c r="G212" s="2" t="s">
         <v>2212</v>
@@ -24590,7 +24568,7 @@
         <v>551</v>
       </c>
       <c r="F213" s="2" t="s">
-        <v>2766</v>
+        <v>2763</v>
       </c>
       <c r="G213" s="2" t="s">
         <v>2213</v>
@@ -24641,10 +24619,10 @@
         <v>605</v>
       </c>
       <c r="F214" s="2" t="s">
-        <v>2767</v>
+        <v>2764</v>
       </c>
       <c r="G214" s="2" t="s">
-        <v>2768</v>
+        <v>2765</v>
       </c>
       <c r="H214" s="2" t="s">
         <v>264</v>
@@ -24692,10 +24670,10 @@
         <v>632</v>
       </c>
       <c r="F215" s="2" t="s">
-        <v>2769</v>
+        <v>2766</v>
       </c>
       <c r="G215" s="2" t="s">
-        <v>2770</v>
+        <v>2767</v>
       </c>
       <c r="H215" s="2" t="s">
         <v>264</v>
@@ -24743,10 +24721,10 @@
         <v>632</v>
       </c>
       <c r="F216" s="2" t="s">
-        <v>2771</v>
+        <v>2768</v>
       </c>
       <c r="G216" s="2" t="s">
-        <v>2772</v>
+        <v>2769</v>
       </c>
       <c r="H216" s="2" t="s">
         <v>264</v>
@@ -24794,10 +24772,10 @@
         <v>787</v>
       </c>
       <c r="F217" s="2" t="s">
-        <v>2773</v>
+        <v>2770</v>
       </c>
       <c r="G217" s="2" t="s">
-        <v>2774</v>
+        <v>2771</v>
       </c>
       <c r="H217" s="2" t="s">
         <v>264</v>
@@ -24845,10 +24823,10 @@
         <v>258</v>
       </c>
       <c r="F218" s="2" t="s">
-        <v>2775</v>
+        <v>2772</v>
       </c>
       <c r="G218" s="2" t="s">
-        <v>2776</v>
+        <v>2773</v>
       </c>
       <c r="H218" s="2" t="s">
         <v>264</v>
@@ -24892,10 +24870,10 @@
         <v>867</v>
       </c>
       <c r="F219" s="2" t="s">
-        <v>2777</v>
+        <v>2774</v>
       </c>
       <c r="G219" s="2" t="s">
-        <v>2778</v>
+        <v>2775</v>
       </c>
       <c r="H219" s="2" t="s">
         <v>264</v>
@@ -24943,7 +24921,7 @@
         <v>1021</v>
       </c>
       <c r="F220" s="2" t="s">
-        <v>2779</v>
+        <v>2776</v>
       </c>
       <c r="G220" s="2" t="s">
         <v>2214</v>
@@ -24994,10 +24972,10 @@
         <v>1074</v>
       </c>
       <c r="F221" s="2" t="s">
-        <v>2780</v>
+        <v>2777</v>
       </c>
       <c r="G221" s="2" t="s">
-        <v>2781</v>
+        <v>2778</v>
       </c>
       <c r="H221" s="2" t="s">
         <v>264</v>
@@ -25045,7 +25023,7 @@
         <v>1170</v>
       </c>
       <c r="F222" s="2" t="s">
-        <v>2782</v>
+        <v>2779</v>
       </c>
       <c r="G222" s="2" t="s">
         <v>2215</v>
@@ -25096,7 +25074,7 @@
         <v>1217</v>
       </c>
       <c r="F223" s="2" t="s">
-        <v>2783</v>
+        <v>2780</v>
       </c>
       <c r="G223" s="2" t="s">
         <v>2216</v>
@@ -25147,10 +25125,10 @@
         <v>258</v>
       </c>
       <c r="F224" s="2" t="s">
-        <v>2784</v>
+        <v>2781</v>
       </c>
       <c r="G224" s="2" t="s">
-        <v>2785</v>
+        <v>2782</v>
       </c>
       <c r="H224" s="2" t="s">
         <v>264</v>
@@ -25198,10 +25176,10 @@
         <v>258</v>
       </c>
       <c r="F225" s="2" t="s">
-        <v>2786</v>
+        <v>2783</v>
       </c>
       <c r="G225" s="2" t="s">
-        <v>2787</v>
+        <v>2784</v>
       </c>
       <c r="H225" s="2" t="s">
         <v>264</v>
@@ -25246,10 +25224,10 @@
         <v>1603</v>
       </c>
       <c r="E226" s="2" t="s">
-        <v>2788</v>
+        <v>2785</v>
       </c>
       <c r="F226" s="2" t="s">
-        <v>2789</v>
+        <v>2786</v>
       </c>
       <c r="G226" s="2" t="s">
         <v>2217</v>
@@ -25293,10 +25271,10 @@
         <v>1616</v>
       </c>
       <c r="E227" s="2" t="s">
-        <v>2790</v>
+        <v>2787</v>
       </c>
       <c r="F227" s="2" t="s">
-        <v>2791</v>
+        <v>2788</v>
       </c>
       <c r="G227" s="2" t="s">
         <v>2218</v>
@@ -25347,10 +25325,10 @@
         <v>1836</v>
       </c>
       <c r="F228" s="2" t="s">
-        <v>2792</v>
+        <v>2789</v>
       </c>
       <c r="G228" s="2" t="s">
-        <v>2793</v>
+        <v>2790</v>
       </c>
       <c r="H228" s="2" t="s">
         <v>264</v>
@@ -25398,7 +25376,7 @@
         <v>1912</v>
       </c>
       <c r="F229" s="2" t="s">
-        <v>2794</v>
+        <v>2791</v>
       </c>
       <c r="G229" s="2" t="s">
         <v>2219</v>
@@ -25446,10 +25424,10 @@
         <v>2063</v>
       </c>
       <c r="E230" s="2" t="s">
-        <v>2795</v>
+        <v>2792</v>
       </c>
       <c r="F230" s="2" t="s">
-        <v>2796</v>
+        <v>2793</v>
       </c>
       <c r="G230" s="2" t="s">
         <v>2220</v>
@@ -25500,10 +25478,10 @@
         <v>258</v>
       </c>
       <c r="F231" s="2" t="s">
-        <v>2797</v>
+        <v>2794</v>
       </c>
       <c r="G231" s="2" t="s">
-        <v>2798</v>
+        <v>2795</v>
       </c>
       <c r="H231" s="2" t="s">
         <v>1153</v>
@@ -25551,10 +25529,10 @@
         <v>1843</v>
       </c>
       <c r="F232" s="2" t="s">
-        <v>2799</v>
+        <v>2796</v>
       </c>
       <c r="G232" s="2" t="s">
-        <v>2800</v>
+        <v>2797</v>
       </c>
       <c r="H232" s="2" t="s">
         <v>1153</v>
@@ -25601,7 +25579,7 @@
         <v>323</v>
       </c>
       <c r="F233" s="2" t="s">
-        <v>2801</v>
+        <v>2798</v>
       </c>
       <c r="G233" s="2" t="s">
         <v>2221</v>
@@ -25640,7 +25618,7 @@
         <v>2179</v>
       </c>
       <c r="S233" s="2" t="s">
-        <v>2892</v>
+        <v>2889</v>
       </c>
     </row>
     <row r="234" spans="1:19" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -25660,7 +25638,7 @@
         <v>832</v>
       </c>
       <c r="F234" s="2" t="s">
-        <v>2802</v>
+        <v>2799</v>
       </c>
       <c r="G234" s="2" t="s">
         <v>2222</v>
@@ -25699,7 +25677,7 @@
         <v>2179</v>
       </c>
       <c r="S234" s="2" t="s">
-        <v>2889</v>
+        <v>2886</v>
       </c>
     </row>
     <row r="235" spans="1:19" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -25719,7 +25697,7 @@
         <v>1183</v>
       </c>
       <c r="F235" s="2" t="s">
-        <v>2803</v>
+        <v>2800</v>
       </c>
       <c r="G235" s="2" t="s">
         <v>2223</v>
@@ -25758,7 +25736,7 @@
         <v>2179</v>
       </c>
       <c r="S235" s="2" t="s">
-        <v>2917</v>
+        <v>2913</v>
       </c>
     </row>
     <row r="236" spans="1:19" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -25778,7 +25756,7 @@
         <v>1196</v>
       </c>
       <c r="F236" s="2" t="s">
-        <v>2804</v>
+        <v>2801</v>
       </c>
       <c r="G236" s="2" t="s">
         <v>2224</v>
@@ -25817,7 +25795,7 @@
         <v>2179</v>
       </c>
       <c r="S236" s="2" t="s">
-        <v>2915</v>
+        <v>2911</v>
       </c>
     </row>
     <row r="237" spans="1:19" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -25837,7 +25815,7 @@
         <v>1417</v>
       </c>
       <c r="F237" s="2" t="s">
-        <v>2805</v>
+        <v>2802</v>
       </c>
       <c r="G237" s="2" t="s">
         <v>2225</v>
@@ -25876,7 +25854,7 @@
         <v>2179</v>
       </c>
       <c r="S237" s="2" t="s">
-        <v>2888</v>
+        <v>2885</v>
       </c>
     </row>
     <row r="238" spans="1:19" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -25896,7 +25874,7 @@
         <v>1491</v>
       </c>
       <c r="F238" s="2" t="s">
-        <v>2806</v>
+        <v>2803</v>
       </c>
       <c r="G238" s="2" t="s">
         <v>2226</v>
@@ -25935,7 +25913,7 @@
         <v>2179</v>
       </c>
       <c r="S238" s="2" t="s">
-        <v>2916</v>
+        <v>2912</v>
       </c>
     </row>
     <row r="239" spans="1:19" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -25952,10 +25930,10 @@
         <v>540</v>
       </c>
       <c r="F239" s="2" t="s">
-        <v>2807</v>
+        <v>2804</v>
       </c>
       <c r="G239" s="2" t="s">
-        <v>2808</v>
+        <v>2805</v>
       </c>
       <c r="H239" s="2" t="s">
         <v>1741</v>
@@ -26002,7 +25980,7 @@
         <v>540</v>
       </c>
       <c r="F240" s="2" t="s">
-        <v>2809</v>
+        <v>2806</v>
       </c>
       <c r="G240" s="2" t="s">
         <v>2227</v>
@@ -26052,7 +26030,7 @@
         <v>540</v>
       </c>
       <c r="F241" s="2" t="s">
-        <v>2810</v>
+        <v>2807</v>
       </c>
       <c r="G241" s="2" t="s">
         <v>2228</v>
@@ -26102,7 +26080,7 @@
         <v>794</v>
       </c>
       <c r="F242" s="2" t="s">
-        <v>2811</v>
+        <v>2808</v>
       </c>
       <c r="G242" s="2" t="s">
         <v>2229</v>
@@ -26152,7 +26130,7 @@
         <v>1424</v>
       </c>
       <c r="F243" s="2" t="s">
-        <v>2812</v>
+        <v>2809</v>
       </c>
       <c r="G243" s="2" t="s">
         <v>2230</v>
@@ -26202,7 +26180,7 @@
         <v>540</v>
       </c>
       <c r="F244" s="2" t="s">
-        <v>2813</v>
+        <v>2810</v>
       </c>
       <c r="G244" s="2" t="s">
         <v>2231</v>
@@ -26256,10 +26234,10 @@
         <v>313</v>
       </c>
       <c r="F245" s="2" t="s">
-        <v>2814</v>
+        <v>2811</v>
       </c>
       <c r="G245" s="2" t="s">
-        <v>2815</v>
+        <v>2812</v>
       </c>
       <c r="H245" s="2" t="s">
         <v>319</v>
@@ -26303,10 +26281,10 @@
         <v>1034</v>
       </c>
       <c r="F246" s="2" t="s">
-        <v>2816</v>
+        <v>2813</v>
       </c>
       <c r="G246" s="2" t="s">
-        <v>2817</v>
+        <v>2814</v>
       </c>
       <c r="H246" s="2" t="s">
         <v>319</v>
@@ -26353,7 +26331,7 @@
         <v>942</v>
       </c>
       <c r="F247" s="2" t="s">
-        <v>2818</v>
+        <v>2815</v>
       </c>
       <c r="G247" s="2" t="s">
         <v>2232</v>
@@ -26389,7 +26367,7 @@
         <v>2179</v>
       </c>
       <c r="S247" s="2" t="s">
-        <v>2904</v>
+        <v>2900</v>
       </c>
     </row>
     <row r="248" spans="1:20" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -26409,7 +26387,7 @@
         <v>2024</v>
       </c>
       <c r="F248" s="2" t="s">
-        <v>2819</v>
+        <v>2816</v>
       </c>
       <c r="G248" s="2" t="s">
         <v>2233</v>
@@ -26463,10 +26441,10 @@
         <v>1761</v>
       </c>
       <c r="F249" s="4" t="s">
-        <v>2820</v>
+        <v>2817</v>
       </c>
       <c r="G249" s="4" t="s">
-        <v>2379</v>
+        <v>2376</v>
       </c>
       <c r="H249" s="2" t="s">
         <v>1767</v>
@@ -26496,10 +26474,10 @@
         <v>9</v>
       </c>
       <c r="S249" s="2" t="s">
-        <v>2374</v>
+        <v>2371</v>
       </c>
       <c r="T249" s="2" t="s">
-        <v>2371</v>
+        <v>2368</v>
       </c>
     </row>
     <row r="250" spans="1:20" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -26520,7 +26498,7 @@
         <v>814</v>
       </c>
       <c r="F250" s="2" t="s">
-        <v>2821</v>
+        <v>2818</v>
       </c>
       <c r="G250" s="2" t="s">
         <v>2234</v>
@@ -26574,7 +26552,7 @@
         <v>971</v>
       </c>
       <c r="F251" s="2" t="s">
-        <v>2822</v>
+        <v>2819</v>
       </c>
       <c r="G251" s="2" t="s">
         <v>2235</v>
@@ -26619,16 +26597,16 @@
         <v>0.5</v>
       </c>
       <c r="D252" s="4" t="s">
-        <v>2398</v>
+        <v>2395</v>
       </c>
       <c r="E252" s="2" t="s">
         <v>1955</v>
       </c>
       <c r="F252" s="4" t="s">
-        <v>2882</v>
+        <v>2879</v>
       </c>
       <c r="G252" s="4" t="s">
-        <v>2883</v>
+        <v>2880</v>
       </c>
       <c r="H252" s="2" t="s">
         <v>977</v>
@@ -26658,7 +26636,7 @@
         <v>9</v>
       </c>
       <c r="S252" s="2" t="s">
-        <v>2397</v>
+        <v>2394</v>
       </c>
     </row>
     <row r="253" spans="1:20" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -26679,7 +26657,7 @@
         <v>1109</v>
       </c>
       <c r="F253" s="2" t="s">
-        <v>2823</v>
+        <v>2820</v>
       </c>
       <c r="G253" s="2" t="s">
         <v>2236</v>
@@ -26730,7 +26708,7 @@
         <v>1402</v>
       </c>
       <c r="F254" s="2" t="s">
-        <v>2824</v>
+        <v>2821</v>
       </c>
       <c r="G254" s="2" t="s">
         <v>2237</v>
@@ -26781,7 +26759,7 @@
         <v>2147</v>
       </c>
       <c r="F255" s="2" t="s">
-        <v>2825</v>
+        <v>2822</v>
       </c>
       <c r="G255" s="2" t="s">
         <v>2238</v>
@@ -26828,10 +26806,10 @@
         <v>69</v>
       </c>
       <c r="F256" s="2" t="s">
-        <v>2826</v>
+        <v>2823</v>
       </c>
       <c r="G256" s="2" t="s">
-        <v>2827</v>
+        <v>2824</v>
       </c>
       <c r="H256" s="2" t="s">
         <v>75</v>
@@ -26876,13 +26854,13 @@
         <v>1163</v>
       </c>
       <c r="E257" s="2" t="s">
-        <v>2828</v>
+        <v>2825</v>
       </c>
       <c r="F257" s="2" t="s">
-        <v>2829</v>
+        <v>2826</v>
       </c>
       <c r="G257" s="2" t="s">
-        <v>2830</v>
+        <v>2827</v>
       </c>
       <c r="H257" s="2" t="s">
         <v>75</v>
@@ -26930,7 +26908,7 @@
         <v>1367</v>
       </c>
       <c r="F258" s="2" t="s">
-        <v>2831</v>
+        <v>2828</v>
       </c>
       <c r="G258" s="2" t="s">
         <v>2239</v>
@@ -26981,7 +26959,7 @@
         <v>2138</v>
       </c>
       <c r="F259" s="2" t="s">
-        <v>2832</v>
+        <v>2829</v>
       </c>
       <c r="G259" s="2" t="s">
         <v>2240</v>
@@ -27026,16 +27004,16 @@
         <v>0.5</v>
       </c>
       <c r="D260" s="4" t="s">
-        <v>2395</v>
+        <v>2392</v>
       </c>
       <c r="E260" s="4" t="s">
-        <v>2394</v>
+        <v>2391</v>
       </c>
       <c r="F260" s="4" t="s">
-        <v>2833</v>
+        <v>2830</v>
       </c>
       <c r="G260" s="4" t="s">
-        <v>2396</v>
+        <v>2393</v>
       </c>
       <c r="H260" s="2" t="s">
         <v>1750</v>
@@ -27065,10 +27043,10 @@
         <v>9</v>
       </c>
       <c r="S260" s="2" t="s">
-        <v>2393</v>
+        <v>2390</v>
       </c>
       <c r="T260" s="2" t="s">
-        <v>2371</v>
+        <v>2368</v>
       </c>
     </row>
     <row r="261" spans="1:20" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -27085,7 +27063,7 @@
         <v>540</v>
       </c>
       <c r="F261" s="6" t="s">
-        <v>2902</v>
+        <v>2898</v>
       </c>
       <c r="G261" s="6" t="s">
         <v>2273</v>
@@ -27121,7 +27099,7 @@
         <v>2183</v>
       </c>
       <c r="S261" s="12" t="s">
-        <v>2903</v>
+        <v>2899</v>
       </c>
       <c r="T261" s="8"/>
     </row>
@@ -27143,7 +27121,7 @@
         <v>1648</v>
       </c>
       <c r="F262" s="9" t="s">
-        <v>2834</v>
+        <v>2831</v>
       </c>
       <c r="G262" s="9" t="s">
         <v>2241</v>
@@ -27179,7 +27157,7 @@
         <v>2183</v>
       </c>
       <c r="S262" s="2" t="s">
-        <v>2903</v>
+        <v>2899</v>
       </c>
     </row>
     <row r="263" spans="1:20" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -27196,7 +27174,7 @@
         <v>2037</v>
       </c>
       <c r="F263" s="2" t="s">
-        <v>2835</v>
+        <v>2832</v>
       </c>
       <c r="G263" s="2" t="s">
         <v>2242</v>
@@ -27247,10 +27225,10 @@
         <v>2278</v>
       </c>
       <c r="F264" s="7" t="s">
-        <v>2893</v>
+        <v>2890</v>
       </c>
       <c r="G264" s="4" t="s">
-        <v>2894</v>
+        <v>2891</v>
       </c>
       <c r="H264" s="2" t="s">
         <v>201</v>
@@ -27307,10 +27285,10 @@
         <v>2275</v>
       </c>
       <c r="F265" s="4" t="s">
-        <v>2895</v>
+        <v>2946</v>
       </c>
       <c r="G265" s="4" t="s">
-        <v>2896</v>
+        <v>2892</v>
       </c>
       <c r="H265" s="2" t="s">
         <v>201</v>
@@ -27346,7 +27324,7 @@
         <v>2183</v>
       </c>
       <c r="S265" s="2" t="s">
-        <v>2897</v>
+        <v>2893</v>
       </c>
     </row>
     <row r="266" spans="1:20" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -27360,16 +27338,16 @@
         <v>0</v>
       </c>
       <c r="D266" s="11" t="s">
-        <v>2898</v>
+        <v>2894</v>
       </c>
       <c r="E266" s="11" t="s">
-        <v>2899</v>
+        <v>2895</v>
       </c>
       <c r="F266" s="11" t="s">
-        <v>2901</v>
+        <v>2897</v>
       </c>
       <c r="G266" s="11" t="s">
-        <v>2900</v>
+        <v>2896</v>
       </c>
       <c r="H266" s="2" t="s">
         <v>201</v>
@@ -27402,7 +27380,7 @@
         <v>9</v>
       </c>
       <c r="R266" s="10" t="s">
-        <v>2284</v>
+        <v>2283</v>
       </c>
     </row>
     <row r="267" spans="1:20" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -27420,10 +27398,10 @@
         <v>1932</v>
       </c>
       <c r="E267" s="2" t="s">
-        <v>2836</v>
+        <v>2833</v>
       </c>
       <c r="F267" s="2" t="s">
-        <v>2837</v>
+        <v>2834</v>
       </c>
       <c r="G267" s="2" t="s">
         <v>2243</v>
@@ -27471,13 +27449,13 @@
         <v>1040</v>
       </c>
       <c r="E268" s="2" t="s">
-        <v>2838</v>
+        <v>2835</v>
       </c>
       <c r="F268" s="2" t="s">
-        <v>2839</v>
+        <v>2836</v>
       </c>
       <c r="G268" s="2" t="s">
-        <v>2840</v>
+        <v>2837</v>
       </c>
       <c r="H268" s="2" t="s">
         <v>1046</v>
@@ -27525,7 +27503,7 @@
         <v>2070</v>
       </c>
       <c r="F269" s="2" t="s">
-        <v>2841</v>
+        <v>2838</v>
       </c>
       <c r="G269" s="2" t="s">
         <v>2244</v>
@@ -27565,8 +27543,8 @@
       <c r="B270" s="5" t="s">
         <v>2180</v>
       </c>
-      <c r="C270" s="2">
-        <v>0.5</v>
+      <c r="C270" s="7">
+        <v>0</v>
       </c>
       <c r="D270" s="2" t="s">
         <v>156</v>
@@ -27575,7 +27553,7 @@
         <v>157</v>
       </c>
       <c r="F270" s="2" t="s">
-        <v>2842</v>
+        <v>2839</v>
       </c>
       <c r="G270" s="2" t="s">
         <v>2245</v>
@@ -27611,13 +27589,13 @@
         <v>9</v>
       </c>
       <c r="R270" s="5" t="s">
-        <v>2289</v>
+        <v>2286</v>
       </c>
       <c r="S270" s="2" t="s">
-        <v>2378</v>
+        <v>2375</v>
       </c>
       <c r="T270" s="2" t="s">
-        <v>2372</v>
+        <v>2369</v>
       </c>
     </row>
     <row r="271" spans="1:20" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -27627,8 +27605,8 @@
       <c r="B271" s="5" t="s">
         <v>2180</v>
       </c>
-      <c r="C271" s="2">
-        <v>0.5</v>
+      <c r="C271" s="7">
+        <v>0</v>
       </c>
       <c r="D271" s="2" t="s">
         <v>750</v>
@@ -27637,7 +27615,7 @@
         <v>157</v>
       </c>
       <c r="F271" s="2" t="s">
-        <v>2843</v>
+        <v>2840</v>
       </c>
       <c r="G271" s="2" t="s">
         <v>2246</v>
@@ -27673,13 +27651,13 @@
         <v>9</v>
       </c>
       <c r="R271" s="5" t="s">
-        <v>2289</v>
+        <v>2286</v>
       </c>
       <c r="S271" s="2" t="s">
-        <v>2377</v>
+        <v>2374</v>
       </c>
       <c r="T271" s="2" t="s">
-        <v>2372</v>
+        <v>2369</v>
       </c>
     </row>
     <row r="272" spans="1:20" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -27700,7 +27678,7 @@
         <v>1074</v>
       </c>
       <c r="F272" s="2" t="s">
-        <v>2844</v>
+        <v>2841</v>
       </c>
       <c r="G272" s="2" t="s">
         <v>2247</v>
@@ -27751,7 +27729,7 @@
         <v>1683</v>
       </c>
       <c r="F273" s="2" t="s">
-        <v>2845</v>
+        <v>2842</v>
       </c>
       <c r="G273" s="2" t="s">
         <v>2248</v>
@@ -27802,7 +27780,7 @@
         <v>1074</v>
       </c>
       <c r="F274" s="2" t="s">
-        <v>2846</v>
+        <v>2843</v>
       </c>
       <c r="G274" s="2" t="s">
         <v>2249</v>
@@ -27843,16 +27821,16 @@
         <v>0</v>
       </c>
       <c r="D275" s="4" t="s">
-        <v>2884</v>
+        <v>2881</v>
       </c>
       <c r="E275" s="2" t="s">
         <v>1576</v>
       </c>
       <c r="F275" s="4" t="s">
-        <v>2885</v>
+        <v>2882</v>
       </c>
       <c r="G275" s="4" t="s">
-        <v>2886</v>
+        <v>2883</v>
       </c>
       <c r="H275" s="2" t="s">
         <v>1582</v>
@@ -27882,7 +27860,7 @@
         <v>9</v>
       </c>
       <c r="S275" s="2" t="s">
-        <v>2887</v>
+        <v>2884</v>
       </c>
     </row>
     <row r="276" spans="1:19" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -27899,7 +27877,7 @@
         <v>540</v>
       </c>
       <c r="F276" s="2" t="s">
-        <v>2847</v>
+        <v>2844</v>
       </c>
       <c r="G276" s="2" t="s">
         <v>2250</v>
@@ -27950,7 +27928,7 @@
         <v>1504</v>
       </c>
       <c r="F277" s="2" t="s">
-        <v>2848</v>
+        <v>2845</v>
       </c>
       <c r="G277" s="2" t="s">
         <v>2251</v>
@@ -27998,10 +27976,10 @@
         <v>1327</v>
       </c>
       <c r="E278" s="2" t="s">
-        <v>2849</v>
+        <v>2846</v>
       </c>
       <c r="F278" s="2" t="s">
-        <v>2850</v>
+        <v>2847</v>
       </c>
       <c r="G278" s="2" t="s">
         <v>2252</v>
@@ -28055,7 +28033,7 @@
         <v>221</v>
       </c>
       <c r="F279" s="2" t="s">
-        <v>2851</v>
+        <v>2848</v>
       </c>
       <c r="G279" s="2" t="s">
         <v>2253</v>
@@ -28106,10 +28084,10 @@
         <v>359</v>
       </c>
       <c r="F280" s="2" t="s">
-        <v>2852</v>
+        <v>2849</v>
       </c>
       <c r="G280" s="2" t="s">
-        <v>2368</v>
+        <v>2365</v>
       </c>
       <c r="H280" s="2" t="s">
         <v>227</v>
@@ -28157,7 +28135,7 @@
         <v>900</v>
       </c>
       <c r="F281" s="2" t="s">
-        <v>2853</v>
+        <v>2850</v>
       </c>
       <c r="G281" s="2" t="s">
         <v>2254</v>
@@ -28208,7 +28186,7 @@
         <v>1203</v>
       </c>
       <c r="F282" s="2" t="s">
-        <v>2854</v>
+        <v>2851</v>
       </c>
       <c r="G282" s="2" t="s">
         <v>2255</v>
@@ -28259,7 +28237,7 @@
         <v>1464</v>
       </c>
       <c r="F283" s="2" t="s">
-        <v>2855</v>
+        <v>2852</v>
       </c>
       <c r="G283" s="2" t="s">
         <v>2256</v>
@@ -28310,7 +28288,7 @@
         <v>1709</v>
       </c>
       <c r="F284" s="2" t="s">
-        <v>2856</v>
+        <v>2853</v>
       </c>
       <c r="G284" s="2" t="s">
         <v>2257</v>
@@ -28354,13 +28332,13 @@
         <v>2005</v>
       </c>
       <c r="E285" s="2" t="s">
-        <v>2857</v>
+        <v>2854</v>
       </c>
       <c r="F285" s="2" t="s">
-        <v>2858</v>
+        <v>2855</v>
       </c>
       <c r="G285" s="2" t="s">
-        <v>2859</v>
+        <v>2856</v>
       </c>
       <c r="H285" s="2" t="s">
         <v>227</v>
@@ -28404,10 +28382,10 @@
         <v>106</v>
       </c>
       <c r="F286" s="2" t="s">
-        <v>2860</v>
+        <v>2857</v>
       </c>
       <c r="G286" s="2" t="s">
-        <v>2861</v>
+        <v>2858</v>
       </c>
       <c r="H286" s="2" t="s">
         <v>112</v>
@@ -28448,10 +28426,10 @@
         <v>880</v>
       </c>
       <c r="E287" s="2" t="s">
-        <v>2862</v>
+        <v>2859</v>
       </c>
       <c r="F287" s="2" t="s">
-        <v>2863</v>
+        <v>2860</v>
       </c>
       <c r="G287" s="2" t="s">
         <v>2258</v>
@@ -28502,7 +28480,7 @@
         <v>1697</v>
       </c>
       <c r="F288" s="2" t="s">
-        <v>2864</v>
+        <v>2861</v>
       </c>
       <c r="G288" s="2" t="s">
         <v>2259</v>
@@ -28553,7 +28531,7 @@
         <v>1803</v>
       </c>
       <c r="F289" s="2" t="s">
-        <v>2865</v>
+        <v>2862</v>
       </c>
       <c r="G289" s="2" t="s">
         <v>2260</v>
@@ -28604,7 +28582,7 @@
         <v>2098</v>
       </c>
       <c r="F290" s="2" t="s">
-        <v>2866</v>
+        <v>2863</v>
       </c>
       <c r="G290" s="2" t="s">
         <v>2261</v>
@@ -28655,10 +28633,10 @@
         <v>1057</v>
       </c>
       <c r="F291" s="2" t="s">
-        <v>2867</v>
+        <v>2864</v>
       </c>
       <c r="G291" s="2" t="s">
-        <v>2868</v>
+        <v>2865</v>
       </c>
       <c r="H291" s="2" t="s">
         <v>1063</v>
@@ -28702,10 +28680,10 @@
         <v>247</v>
       </c>
       <c r="E292" s="2" t="s">
-        <v>2869</v>
+        <v>2866</v>
       </c>
       <c r="F292" s="2" t="s">
-        <v>2870</v>
+        <v>2867</v>
       </c>
       <c r="G292" s="2" t="s">
         <v>2262</v>
@@ -28762,7 +28740,7 @@
         <v>231</v>
       </c>
       <c r="F293" s="2" t="s">
-        <v>2871</v>
+        <v>2868</v>
       </c>
       <c r="G293" s="2" t="s">
         <v>2263</v>
@@ -28816,7 +28794,7 @@
         <v>612</v>
       </c>
       <c r="F294" s="2" t="s">
-        <v>2872</v>
+        <v>2869</v>
       </c>
       <c r="G294" s="2" t="s">
         <v>2264</v>
@@ -28870,7 +28848,7 @@
         <v>718</v>
       </c>
       <c r="F295" s="2" t="s">
-        <v>2873</v>
+        <v>2870</v>
       </c>
       <c r="G295" s="2" t="s">
         <v>2265</v>
@@ -28924,7 +28902,7 @@
         <v>807</v>
       </c>
       <c r="F296" s="2" t="s">
-        <v>2874</v>
+        <v>2871</v>
       </c>
       <c r="G296" s="2" t="s">
         <v>2266</v>
@@ -28978,7 +28956,7 @@
         <v>825</v>
       </c>
       <c r="F297" s="2" t="s">
-        <v>2875</v>
+        <v>2872</v>
       </c>
       <c r="G297" s="2" t="s">
         <v>2267</v>
@@ -29032,7 +29010,7 @@
         <v>1102</v>
       </c>
       <c r="F298" s="2" t="s">
-        <v>2876</v>
+        <v>2873</v>
       </c>
       <c r="G298" s="2" t="s">
         <v>2268</v>
@@ -29086,7 +29064,7 @@
         <v>1360</v>
       </c>
       <c r="F299" s="2" t="s">
-        <v>2877</v>
+        <v>2874</v>
       </c>
       <c r="G299" s="2" t="s">
         <v>2269</v>
@@ -29136,7 +29114,7 @@
         <v>540</v>
       </c>
       <c r="F300" s="2" t="s">
-        <v>2878</v>
+        <v>2875</v>
       </c>
       <c r="G300" s="2" t="s">
         <v>2270</v>
@@ -29190,7 +29168,7 @@
         <v>1655</v>
       </c>
       <c r="F301" s="2" t="s">
-        <v>2879</v>
+        <v>2876</v>
       </c>
       <c r="G301" s="2" t="s">
         <v>2271</v>
@@ -29244,10 +29222,10 @@
         <v>1132</v>
       </c>
       <c r="F302" s="2" t="s">
-        <v>2880</v>
+        <v>2877</v>
       </c>
       <c r="G302" s="4" t="s">
-        <v>2922</v>
+        <v>2918</v>
       </c>
       <c r="H302" s="2" t="s">
         <v>1138</v>
@@ -29296,7 +29274,7 @@
         <v>1948</v>
       </c>
       <c r="F303" s="2" t="s">
-        <v>2881</v>
+        <v>2878</v>
       </c>
       <c r="G303" s="2" t="s">
         <v>2272</v>
@@ -29341,16 +29319,16 @@
         <v>0.5</v>
       </c>
       <c r="D304" s="4" t="s">
+        <v>2377</v>
+      </c>
+      <c r="E304" s="4" t="s">
+        <v>2378</v>
+      </c>
+      <c r="F304" s="7" t="s">
+        <v>2379</v>
+      </c>
+      <c r="G304" s="7" t="s">
         <v>2380</v>
-      </c>
-      <c r="E304" s="4" t="s">
-        <v>2381</v>
-      </c>
-      <c r="F304" s="7" t="s">
-        <v>2382</v>
-      </c>
-      <c r="G304" s="7" t="s">
-        <v>2383</v>
       </c>
       <c r="H304" s="2" t="s">
         <v>272</v>
@@ -29385,37 +29363,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="78.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>2281</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2285</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2288</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Final changes made with the last 3 controls
Signed-off-by: karikarshivani <karikarshivani@gmail.com>
</commit_message>
<xml_diff>
--- a/cms-ars-3.1-high-microsoft-windows-server-2019-stig-overlay.xlsx
+++ b/cms-ars-3.1-high-microsoft-windows-server-2019-stig-overlay.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shivanik\Desktop\InSpec\Windows\Windows Server 2019\Overlay\High\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shivanik\Desktop\InSpec\Windows\Windows Server 2019\Overlay\High\cms-ars-3.1-high-microsoft-windows-server-2019-stig-overlay\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="27870" windowHeight="13650" tabRatio="220"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="27870" windowHeight="13650" tabRatio="220"/>
   </bookViews>
   <sheets>
     <sheet name="cmsars3.1high_w2019overlay" sheetId="1" r:id="rId1"/>
@@ -12701,86 +12701,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Determine if manually managed application/service accounts exist. If none exist, this is NA. If passwords for manually managed application/service accounts are not changed at least annually or every 60 days and when an administrator with knowledge of the password leaves the organization, this is a finding. Identify manually managed application/service accounts. To determine the date a password was last changed: Domain controllers: Open \"PowerShell\". Enter \"Get-AdUser -Identity [application account name] -Properties PasswordLastSet | FT Name, PasswordLastSet\", where [application account name] is the name of the manually managed application/service account. If the \"PasswordLastSet\" date is more than </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <strike/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>one year</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 60 days </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>old</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, this is a finding. Member servers and standalone systems: Open \"Command Prompt\". Enter 'Net User [application account name] | Find /i \"Password Last Set\"', where [application account name] is the name of the manually managed application/service account. If the \"Password Last Set\" date is more than </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <strike/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>one year</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 60 days</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> old, this is a finding."</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>Verify the effective setting in Local Group Policy Editor. Run \"gpedit.msc\". Navigate to Local Computer Policy &gt;&gt; Computer Configuration &gt;&gt; Windows Settings &gt;&gt; Security Settings &gt;&gt; Account Policies &gt;&gt; Account Lockout Policy. If the \"Reset account lockout counter after\" value is less than</t>
     </r>
     <r>
@@ -13152,6 +13072,129 @@
         <scheme val="minor"/>
       </rPr>
       <t>. Domain accounts can be configured with an account expiration date, under \"Account\" properties. Local accounts can be configured to expire with the command \"Net user [username] /expires:[mm/dd/yyyy]\", where username is the name of the temporary user account. Delete any temporary user accounts that are no longer necessary.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Determine if manually managed application/service accounts exist. If none exist, this is NA. If passwords for manually managed application/service accounts are not changed at least </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>annually or</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>every 60 days and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> when an administrator with knowledge of the password leaves the organization, this is a finding. Identify manually managed application/service accounts. To determine the date a password was last changed: Domain controllers: Open \"PowerShell\". Enter \"Get-AdUser -Identity [application account name] -Properties PasswordLastSet | FT Name, PasswordLastSet\", where [application account name] is the name of the manually managed application/service account. If the \"PasswordLastSet\" date is more than </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>one year</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 60 days </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>old</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, this is a finding. Member servers and standalone systems: Open \"Command Prompt\". Enter 'Net User [application account name] | Find /i \"Password Last Set\"', where [application account name] is the name of the manually managed application/service account. If the \"Password Last Set\" date is more than </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>one year</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 60 days</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> old, this is a finding."</t>
     </r>
   </si>
 </sst>
@@ -13784,16 +13827,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -14069,14 +14103,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:U304"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14170,7 +14203,7 @@
         <v>2284</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="195" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="195" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>990</v>
       </c>
@@ -14224,7 +14257,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="255" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="255" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>413</v>
       </c>
@@ -14275,7 +14308,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>887</v>
       </c>
@@ -14326,7 +14359,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="405" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="405" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>1942</v>
       </c>
@@ -14380,7 +14413,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="405" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="405" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>1288</v>
       </c>
@@ -14434,7 +14467,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="285" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="285" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>574</v>
       </c>
@@ -14488,7 +14521,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>1730</v>
       </c>
@@ -14557,13 +14590,13 @@
         <v>2280</v>
       </c>
       <c r="E9" s="4" t="s">
+        <v>2943</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>2944</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="G9" s="4" t="s">
         <v>2945</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>2946</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>1435</v>
@@ -14620,10 +14653,10 @@
         <v>2407</v>
       </c>
       <c r="F10" s="4" t="s">
+        <v>2941</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>2942</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>2943</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>562</v>
@@ -14656,7 +14689,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="390" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="390" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>583</v>
       </c>
@@ -14710,7 +14743,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="390" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="390" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>685</v>
       </c>
@@ -14764,7 +14797,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="390" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" ht="390" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>242</v>
       </c>
@@ -14818,7 +14851,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="390" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" ht="390" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>207</v>
       </c>
@@ -14872,7 +14905,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="360" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" ht="360" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>1870</v>
       </c>
@@ -14926,7 +14959,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="360" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" ht="360" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>1000</v>
       </c>
@@ -14980,7 +15013,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" ht="150" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>1225</v>
       </c>
@@ -15031,7 +15064,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" ht="150" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>1263</v>
       </c>
@@ -15082,7 +15115,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="270" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" ht="270" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>839</v>
       </c>
@@ -15133,7 +15166,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="180" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" ht="180" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>919</v>
       </c>
@@ -15184,7 +15217,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="255" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" ht="255" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>2105</v>
       </c>
@@ -15235,7 +15268,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="240" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" ht="240" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>1028</v>
       </c>
@@ -15286,7 +15319,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="225" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" ht="225" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>289</v>
       </c>
@@ -15337,7 +15370,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="240" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" ht="240" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>913</v>
       </c>
@@ -15388,7 +15421,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="270" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" ht="270" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>185</v>
       </c>
@@ -15439,7 +15472,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>673</v>
       </c>
@@ -15490,7 +15523,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>151</v>
       </c>
@@ -15541,7 +15574,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="405" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" ht="405" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>301</v>
       </c>
@@ -15592,7 +15625,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>1256</v>
       </c>
@@ -15643,7 +15676,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="240" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" ht="240" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>61</v>
       </c>
@@ -15862,7 +15895,7 @@
         <v>2179</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>1671</v>
       </c>
@@ -15913,7 +15946,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:18" ht="315" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" ht="315" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>2031</v>
       </c>
@@ -15964,7 +15997,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:18" ht="180" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" ht="180" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>1611</v>
       </c>
@@ -16015,7 +16048,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>1857</v>
       </c>
@@ -16066,7 +16099,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>801</v>
       </c>
@@ -16117,7 +16150,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:18" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>907</v>
       </c>
@@ -16168,7 +16201,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:18" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
         <v>1823</v>
       </c>
@@ -16219,7 +16252,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:18" ht="195" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" ht="195" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
         <v>450</v>
       </c>
@@ -16270,7 +16303,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:18" ht="210" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" ht="210" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
         <v>295</v>
       </c>
@@ -16321,7 +16354,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
         <v>93</v>
       </c>
@@ -16372,7 +16405,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:18" ht="240" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" ht="240" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
         <v>875</v>
       </c>
@@ -16423,7 +16456,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:18" ht="210" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" ht="210" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>589</v>
       </c>
@@ -16474,7 +16507,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:18" ht="195" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" ht="195" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
         <v>1558</v>
       </c>
@@ -16525,7 +16558,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:18" ht="240" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" ht="240" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
         <v>366</v>
       </c>
@@ -16576,7 +16609,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:18" ht="240" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" ht="240" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
         <v>2111</v>
       </c>
@@ -16627,7 +16660,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:17" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" ht="165" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
         <v>334</v>
       </c>
@@ -16678,7 +16711,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:17" ht="240" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" ht="240" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
         <v>1009</v>
       </c>
@@ -16729,7 +16762,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:17" ht="255" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" ht="255" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
         <v>925</v>
       </c>
@@ -16780,7 +16813,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:17" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" ht="165" x14ac:dyDescent="0.25">
       <c r="A52" s="13" t="s">
         <v>2126</v>
       </c>
@@ -16831,7 +16864,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:17" ht="195" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" ht="195" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
         <v>191</v>
       </c>
@@ -16882,7 +16915,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:17" ht="255" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" ht="255" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
         <v>11</v>
       </c>
@@ -16933,7 +16966,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:17" ht="180" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" ht="180" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
         <v>1564</v>
       </c>
@@ -16984,7 +17017,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:17" ht="240" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" ht="240" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
         <v>566</v>
       </c>
@@ -17035,7 +17068,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:17" ht="270" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" ht="270" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
         <v>145</v>
       </c>
@@ -17086,7 +17119,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:17" ht="240" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" ht="240" x14ac:dyDescent="0.25">
       <c r="A58" s="13" t="s">
         <v>38</v>
       </c>
@@ -17137,7 +17170,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:17" ht="195" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" ht="195" x14ac:dyDescent="0.25">
       <c r="A59" s="13" t="s">
         <v>1512</v>
       </c>
@@ -17188,7 +17221,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:17" ht="210" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" ht="210" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
         <v>1084</v>
       </c>
@@ -17239,7 +17272,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:17" ht="225" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" ht="225" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
         <v>469</v>
       </c>
@@ -17290,7 +17323,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:17" ht="210" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" ht="210" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
         <v>1241</v>
       </c>
@@ -17341,7 +17374,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:17" ht="195" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" ht="195" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
         <v>2058</v>
       </c>
@@ -17392,7 +17425,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:17" ht="240" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" ht="240" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="s">
         <v>1677</v>
       </c>
@@ -17443,7 +17476,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:17" ht="240" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" ht="240" x14ac:dyDescent="0.25">
       <c r="A65" s="13" t="s">
         <v>1552</v>
       </c>
@@ -17494,7 +17527,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:17" ht="390" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" ht="390" x14ac:dyDescent="0.25">
       <c r="A66" s="13" t="s">
         <v>626</v>
       </c>
@@ -17548,7 +17581,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:17" ht="360" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" ht="360" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="s">
         <v>1810</v>
       </c>
@@ -17602,7 +17635,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:17" ht="345" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" ht="345" x14ac:dyDescent="0.25">
       <c r="A68" s="13" t="s">
         <v>1309</v>
       </c>
@@ -17656,7 +17689,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:17" ht="345" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" ht="345" x14ac:dyDescent="0.25">
       <c r="A69" s="13" t="s">
         <v>1119</v>
       </c>
@@ -17710,7 +17743,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:17" ht="390" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" ht="390" x14ac:dyDescent="0.25">
       <c r="A70" s="13" t="s">
         <v>861</v>
       </c>
@@ -17764,7 +17797,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:17" ht="375" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" ht="375" x14ac:dyDescent="0.25">
       <c r="A71" s="13" t="s">
         <v>169</v>
       </c>
@@ -17818,7 +17851,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:17" ht="405" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" ht="405" x14ac:dyDescent="0.25">
       <c r="A72" s="13" t="s">
         <v>1546</v>
       </c>
@@ -17872,7 +17905,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:17" ht="405" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" ht="405" x14ac:dyDescent="0.25">
       <c r="A73" s="13" t="s">
         <v>386</v>
       </c>
@@ -17926,7 +17959,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:17" ht="360" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" ht="360" x14ac:dyDescent="0.25">
       <c r="A74" s="13" t="s">
         <v>1994</v>
       </c>
@@ -17980,7 +18013,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:17" ht="360" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" ht="360" x14ac:dyDescent="0.25">
       <c r="A75" s="13" t="s">
         <v>2086</v>
       </c>
@@ -18034,7 +18067,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:17" ht="375" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" ht="375" x14ac:dyDescent="0.25">
       <c r="A76" s="13" t="s">
         <v>1968</v>
       </c>
@@ -18088,7 +18121,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:17" ht="375" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" ht="375" x14ac:dyDescent="0.25">
       <c r="A77" s="13" t="s">
         <v>2092</v>
       </c>
@@ -18142,7 +18175,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:17" ht="375" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" ht="375" x14ac:dyDescent="0.25">
       <c r="A78" s="13" t="s">
         <v>1791</v>
       </c>
@@ -18196,7 +18229,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="1:17" ht="375" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" ht="375" x14ac:dyDescent="0.25">
       <c r="A79" s="13" t="s">
         <v>2012</v>
       </c>
@@ -18250,7 +18283,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="1:17" ht="360" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" ht="360" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="s">
         <v>711</v>
       </c>
@@ -18304,7 +18337,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="81" spans="1:20" ht="360" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:20" ht="360" x14ac:dyDescent="0.25">
       <c r="A81" s="13" t="s">
         <v>1797</v>
       </c>
@@ -18358,7 +18391,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="82" spans="1:20" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:20" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A82" s="13" t="s">
         <v>1390</v>
       </c>
@@ -18412,7 +18445,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:20" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:20" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A83" s="13" t="s">
         <v>1906</v>
       </c>
@@ -18466,7 +18499,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:20" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:20" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A84" s="13" t="s">
         <v>1269</v>
       </c>
@@ -18520,7 +18553,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:20" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:20" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="s">
         <v>725</v>
       </c>
@@ -18574,7 +18607,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:20" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:20" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A86" s="13" t="s">
         <v>1540</v>
       </c>
@@ -18628,7 +18661,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:20" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:20" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A87" s="13" t="s">
         <v>645</v>
       </c>
@@ -18682,7 +18715,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="88" spans="1:20" ht="360" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:20" ht="360" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="s">
         <v>1411</v>
       </c>
@@ -18736,7 +18769,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="89" spans="1:20" ht="360" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:20" ht="360" x14ac:dyDescent="0.25">
       <c r="A89" s="13" t="s">
         <v>2044</v>
       </c>
@@ -18790,7 +18823,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:20" ht="375" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:20" ht="375" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="s">
         <v>526</v>
       </c>
@@ -18844,7 +18877,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:20" ht="375" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:20" ht="375" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="s">
         <v>1592</v>
       </c>
@@ -18898,7 +18931,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:20" ht="240" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:20" ht="240" x14ac:dyDescent="0.25">
       <c r="A92" s="13" t="s">
         <v>597</v>
       </c>
@@ -18967,7 +19000,7 @@
         <v>1523</v>
       </c>
       <c r="F93" s="4" t="s">
-        <v>2941</v>
+        <v>2940</v>
       </c>
       <c r="G93" s="4" t="s">
         <v>2388</v>
@@ -19177,7 +19210,7 @@
         <v>2899</v>
       </c>
     </row>
-    <row r="97" spans="1:17" ht="345" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17" ht="345" x14ac:dyDescent="0.25">
       <c r="A97" s="13" t="s">
         <v>1346</v>
       </c>
@@ -19228,7 +19261,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:17" ht="375" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17" ht="375" x14ac:dyDescent="0.25">
       <c r="A98" s="13" t="s">
         <v>952</v>
       </c>
@@ -19279,7 +19312,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:17" ht="375" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17" ht="375" x14ac:dyDescent="0.25">
       <c r="A99" s="13" t="s">
         <v>2080</v>
       </c>
@@ -19330,7 +19363,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:17" ht="360" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:17" ht="360" x14ac:dyDescent="0.25">
       <c r="A100" s="13" t="s">
         <v>30</v>
       </c>
@@ -19381,7 +19414,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:17" ht="360" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:17" ht="360" x14ac:dyDescent="0.25">
       <c r="A101" s="13" t="s">
         <v>276</v>
       </c>
@@ -19432,7 +19465,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:17" ht="375" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:17" ht="375" x14ac:dyDescent="0.25">
       <c r="A102" s="13" t="s">
         <v>462</v>
       </c>
@@ -19486,7 +19519,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:17" ht="375" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:17" ht="375" x14ac:dyDescent="0.25">
       <c r="A103" s="13" t="s">
         <v>1281</v>
       </c>
@@ -19537,7 +19570,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:17" ht="375" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:17" ht="375" x14ac:dyDescent="0.25">
       <c r="A104" s="13" t="s">
         <v>45</v>
       </c>
@@ -19588,7 +19621,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:17" ht="390" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:17" ht="390" x14ac:dyDescent="0.25">
       <c r="A105" s="13" t="s">
         <v>340</v>
       </c>
@@ -19639,7 +19672,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:17" ht="390" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:17" ht="390" x14ac:dyDescent="0.25">
       <c r="A106" s="13" t="s">
         <v>661</v>
       </c>
@@ -19690,7 +19723,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:17" ht="405" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:17" ht="405" x14ac:dyDescent="0.25">
       <c r="A107" s="13" t="s">
         <v>652</v>
       </c>
@@ -19744,7 +19777,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:17" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A108" s="13" t="s">
         <v>116</v>
       </c>
@@ -19795,7 +19828,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="109" spans="1:17" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A109" s="13" t="s">
         <v>52</v>
       </c>
@@ -19846,7 +19879,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:17" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:17" ht="120" x14ac:dyDescent="0.25">
       <c r="A110" s="13" t="s">
         <v>667</v>
       </c>
@@ -19897,7 +19930,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:17" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:17" ht="120" x14ac:dyDescent="0.25">
       <c r="A111" s="13" t="s">
         <v>1900</v>
       </c>
@@ -19948,7 +19981,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:17" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:17" ht="120" x14ac:dyDescent="0.25">
       <c r="A112" s="13" t="s">
         <v>511</v>
       </c>
@@ -20159,7 +20192,7 @@
         <v>2934</v>
       </c>
     </row>
-    <row r="116" spans="1:20" ht="255" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:20" ht="255" x14ac:dyDescent="0.25">
       <c r="A116" s="13" t="s">
         <v>1975</v>
       </c>
@@ -20213,7 +20246,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="1:20" ht="285" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:20" ht="285" x14ac:dyDescent="0.25">
       <c r="A117" s="13" t="s">
         <v>965</v>
       </c>
@@ -20267,7 +20300,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:20" ht="255" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:20" ht="255" x14ac:dyDescent="0.25">
       <c r="A118" s="13" t="s">
         <v>933</v>
       </c>
@@ -20321,7 +20354,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:20" ht="315" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:20" ht="315" x14ac:dyDescent="0.25">
       <c r="A119" s="13" t="s">
         <v>403</v>
       </c>
@@ -20375,7 +20408,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:20" ht="270" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:20" ht="270" x14ac:dyDescent="0.25">
       <c r="A120" s="13" t="s">
         <v>2117</v>
       </c>
@@ -20594,7 +20627,7 @@
         <v>2179</v>
       </c>
     </row>
-    <row r="124" spans="1:20" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:20" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A124" s="13" t="s">
         <v>1623</v>
       </c>
@@ -20645,7 +20678,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:20" ht="225" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:20" ht="225" x14ac:dyDescent="0.25">
       <c r="A125" s="13" t="s">
         <v>705</v>
       </c>
@@ -20714,7 +20747,7 @@
         <v>1999</v>
       </c>
       <c r="F126" s="4" t="s">
-        <v>2940</v>
+        <v>2946</v>
       </c>
       <c r="G126" s="4" t="s">
         <v>2939</v>
@@ -20753,7 +20786,7 @@
         <v>2370</v>
       </c>
     </row>
-    <row r="127" spans="1:20" ht="390" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:20" ht="390" x14ac:dyDescent="0.25">
       <c r="A127" s="13" t="s">
         <v>1096</v>
       </c>
@@ -20804,7 +20837,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:20" ht="255" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:20" ht="255" x14ac:dyDescent="0.25">
       <c r="A128" s="13" t="s">
         <v>1472</v>
       </c>
@@ -20855,7 +20888,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="129" spans="1:17" ht="180" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:17" ht="180" x14ac:dyDescent="0.25">
       <c r="A129" s="13" t="s">
         <v>87</v>
       </c>
@@ -20906,7 +20939,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="130" spans="1:17" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:17" ht="150" x14ac:dyDescent="0.25">
       <c r="A130" s="13" t="s">
         <v>774</v>
       </c>
@@ -20957,7 +20990,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="131" spans="1:17" ht="225" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:17" ht="225" x14ac:dyDescent="0.25">
       <c r="A131" s="13" t="s">
         <v>732</v>
       </c>
@@ -21008,7 +21041,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="132" spans="1:17" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:17" ht="105" x14ac:dyDescent="0.25">
       <c r="A132" s="13" t="s">
         <v>1920</v>
       </c>
@@ -21059,7 +21092,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="133" spans="1:17" ht="240" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:17" ht="240" x14ac:dyDescent="0.25">
       <c r="A133" s="13" t="s">
         <v>346</v>
       </c>
@@ -21110,7 +21143,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="134" spans="1:17" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:17" ht="165" x14ac:dyDescent="0.25">
       <c r="A134" s="13" t="s">
         <v>781</v>
       </c>
@@ -21161,7 +21194,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="135" spans="1:17" ht="330" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:17" ht="330" x14ac:dyDescent="0.25">
       <c r="A135" s="13" t="s">
         <v>1772</v>
       </c>
@@ -21212,7 +21245,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="136" spans="1:17" ht="225" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:17" ht="225" x14ac:dyDescent="0.25">
       <c r="A136" s="13" t="s">
         <v>2164</v>
       </c>
@@ -21263,7 +21296,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="137" spans="1:17" ht="195" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:17" ht="195" x14ac:dyDescent="0.25">
       <c r="A137" s="13" t="s">
         <v>21</v>
       </c>
@@ -21314,7 +21347,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="138" spans="1:17" ht="225" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:17" ht="225" x14ac:dyDescent="0.25">
       <c r="A138" s="13" t="s">
         <v>1068</v>
       </c>
@@ -21365,7 +21398,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="139" spans="1:17" ht="225" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:17" ht="225" x14ac:dyDescent="0.25">
       <c r="A139" s="13" t="s">
         <v>1534</v>
       </c>
@@ -21416,7 +21449,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="140" spans="1:17" ht="210" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:17" ht="210" x14ac:dyDescent="0.25">
       <c r="A140" s="13" t="s">
         <v>100</v>
       </c>
@@ -21467,7 +21500,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="141" spans="1:17" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:17" ht="120" x14ac:dyDescent="0.25">
       <c r="A141" s="13" t="s">
         <v>894</v>
       </c>
@@ -21518,7 +21551,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="142" spans="1:17" ht="225" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:17" ht="225" x14ac:dyDescent="0.25">
       <c r="A142" s="13" t="s">
         <v>283</v>
       </c>
@@ -21569,7 +21602,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="143" spans="1:17" ht="255" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:17" ht="255" x14ac:dyDescent="0.25">
       <c r="A143" s="13" t="s">
         <v>1485</v>
       </c>
@@ -21620,7 +21653,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="144" spans="1:17" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:17" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A144" s="13" t="s">
         <v>496</v>
       </c>
@@ -21671,7 +21704,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="145" spans="1:17" ht="210" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:17" ht="210" x14ac:dyDescent="0.25">
       <c r="A145" s="13" t="s">
         <v>1571</v>
       </c>
@@ -21722,7 +21755,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="146" spans="1:17" ht="315" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:17" ht="315" x14ac:dyDescent="0.25">
       <c r="A146" s="13" t="s">
         <v>1211</v>
       </c>
@@ -21773,7 +21806,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="147" spans="1:17" ht="195" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:17" ht="195" x14ac:dyDescent="0.25">
       <c r="A147" s="13" t="s">
         <v>1339</v>
       </c>
@@ -21824,7 +21857,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="148" spans="1:17" ht="195" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:17" ht="195" x14ac:dyDescent="0.25">
       <c r="A148" s="13" t="s">
         <v>1988</v>
       </c>
@@ -21875,7 +21908,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="149" spans="1:17" ht="330" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:17" ht="330" x14ac:dyDescent="0.25">
       <c r="A149" s="13" t="s">
         <v>1158</v>
       </c>
@@ -21926,7 +21959,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="150" spans="1:17" ht="240" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:17" ht="240" x14ac:dyDescent="0.25">
       <c r="A150" s="13" t="s">
         <v>1877</v>
       </c>
@@ -21977,7 +22010,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="151" spans="1:17" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:17" ht="135" x14ac:dyDescent="0.25">
       <c r="A151" s="13" t="s">
         <v>1126</v>
       </c>
@@ -22028,7 +22061,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="152" spans="1:17" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:17" ht="135" x14ac:dyDescent="0.25">
       <c r="A152" s="13" t="s">
         <v>1927</v>
       </c>
@@ -22079,7 +22112,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="153" spans="1:17" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:17" ht="105" x14ac:dyDescent="0.25">
       <c r="A153" s="13" t="s">
         <v>758</v>
       </c>
@@ -22130,7 +22163,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="154" spans="1:17" ht="180" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:17" ht="180" x14ac:dyDescent="0.25">
       <c r="A154" s="13" t="s">
         <v>1894</v>
       </c>
@@ -22181,7 +22214,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="155" spans="1:17" ht="180" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:17" ht="180" x14ac:dyDescent="0.25">
       <c r="A155" s="13" t="s">
         <v>1664</v>
       </c>
@@ -22232,7 +22265,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="156" spans="1:17" ht="285" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:17" ht="285" x14ac:dyDescent="0.25">
       <c r="A156" s="13" t="s">
         <v>958</v>
       </c>
@@ -22279,7 +22312,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="157" spans="1:17" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:17" ht="105" x14ac:dyDescent="0.25">
       <c r="A157" s="13" t="s">
         <v>1478</v>
       </c>
@@ -22326,7 +22359,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="158" spans="1:17" ht="300" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:17" ht="300" x14ac:dyDescent="0.25">
       <c r="A158" s="13" t="s">
         <v>1051</v>
       </c>
@@ -22373,7 +22406,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="159" spans="1:17" ht="345" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:17" ht="345" x14ac:dyDescent="0.25">
       <c r="A159" s="13" t="s">
         <v>739</v>
       </c>
@@ -22424,7 +22457,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="160" spans="1:17" ht="225" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:17" ht="225" x14ac:dyDescent="0.25">
       <c r="A160" s="13" t="s">
         <v>1830</v>
       </c>
@@ -22475,7 +22508,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="161" spans="1:19" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:19" ht="135" x14ac:dyDescent="0.25">
       <c r="A161" s="13" t="s">
         <v>1451</v>
       </c>
@@ -22526,7 +22559,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="162" spans="1:19" ht="180" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:19" ht="180" x14ac:dyDescent="0.25">
       <c r="A162" s="13" t="s">
         <v>534</v>
       </c>
@@ -22631,7 +22664,7 @@
         <v>2890</v>
       </c>
     </row>
-    <row r="164" spans="1:19" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:19" ht="150" x14ac:dyDescent="0.25">
       <c r="A164" s="13" t="s">
         <v>1458</v>
       </c>
@@ -22682,7 +22715,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="165" spans="1:19" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:19" ht="105" x14ac:dyDescent="0.25">
       <c r="A165" s="13" t="s">
         <v>179</v>
       </c>
@@ -22733,7 +22766,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="166" spans="1:19" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:19" ht="120" x14ac:dyDescent="0.25">
       <c r="A166" s="13" t="s">
         <v>80</v>
       </c>
@@ -22784,7 +22817,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="167" spans="1:19" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:19" ht="150" x14ac:dyDescent="0.25">
       <c r="A167" s="13" t="s">
         <v>1851</v>
       </c>
@@ -22835,7 +22868,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="168" spans="1:19" ht="210" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:19" ht="210" x14ac:dyDescent="0.25">
       <c r="A168" s="13" t="s">
         <v>476</v>
       </c>
@@ -22886,7 +22919,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="169" spans="1:19" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:19" ht="90" x14ac:dyDescent="0.25">
       <c r="A169" s="13" t="s">
         <v>520</v>
       </c>
@@ -22937,7 +22970,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="170" spans="1:19" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:19" ht="135" x14ac:dyDescent="0.25">
       <c r="A170" s="13" t="s">
         <v>1691</v>
       </c>
@@ -22988,7 +23021,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="171" spans="1:19" ht="240" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:19" ht="240" x14ac:dyDescent="0.25">
       <c r="A171" s="13" t="s">
         <v>353</v>
       </c>
@@ -23039,7 +23072,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="172" spans="1:19" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:19" ht="120" x14ac:dyDescent="0.25">
       <c r="A172" s="13" t="s">
         <v>1785</v>
       </c>
@@ -23090,7 +23123,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="173" spans="1:19" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:19" ht="150" x14ac:dyDescent="0.25">
       <c r="A173" s="13" t="s">
         <v>503</v>
       </c>
@@ -23141,7 +23174,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="174" spans="1:19" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:19" ht="150" x14ac:dyDescent="0.25">
       <c r="A174" s="13" t="s">
         <v>1444</v>
       </c>
@@ -23192,7 +23225,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="175" spans="1:19" ht="255" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:19" ht="255" x14ac:dyDescent="0.25">
       <c r="A175" s="13" t="s">
         <v>489</v>
       </c>
@@ -23243,7 +23276,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="176" spans="1:19" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:19" ht="150" x14ac:dyDescent="0.25">
       <c r="A176" s="13" t="s">
         <v>1864</v>
       </c>
@@ -24750,7 +24783,7 @@
       </c>
       <c r="S204" s="11"/>
     </row>
-    <row r="205" spans="1:19" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:19" ht="165" x14ac:dyDescent="0.25">
       <c r="A205" s="13" t="s">
         <v>692</v>
       </c>
@@ -24797,7 +24830,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="206" spans="1:19" ht="195" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:19" ht="195" x14ac:dyDescent="0.25">
       <c r="A206" s="13" t="s">
         <v>1755</v>
       </c>
@@ -24848,7 +24881,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="207" spans="1:19" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:19" ht="120" x14ac:dyDescent="0.25">
       <c r="A207" s="13" t="s">
         <v>853</v>
       </c>
@@ -24899,7 +24932,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="208" spans="1:19" ht="240" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:19" ht="240" x14ac:dyDescent="0.25">
       <c r="A208" s="13" t="s">
         <v>1303</v>
       </c>
@@ -24950,7 +24983,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="209" spans="1:20" ht="315" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:20" ht="315" x14ac:dyDescent="0.25">
       <c r="A209" s="13" t="s">
         <v>1248</v>
       </c>
@@ -25007,7 +25040,7 @@
         <v>2373</v>
       </c>
     </row>
-    <row r="210" spans="1:20" ht="180" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:20" ht="180" x14ac:dyDescent="0.25">
       <c r="A210" s="13" t="s">
         <v>552</v>
       </c>
@@ -25058,7 +25091,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="211" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:20" ht="165" x14ac:dyDescent="0.25">
       <c r="A211" s="13" t="s">
         <v>260</v>
       </c>
@@ -25109,7 +25142,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="212" spans="1:20" ht="180" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:20" ht="180" x14ac:dyDescent="0.25">
       <c r="A212" s="13" t="s">
         <v>1275</v>
       </c>
@@ -25160,7 +25193,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="213" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:20" ht="165" x14ac:dyDescent="0.25">
       <c r="A213" s="13" t="s">
         <v>845</v>
       </c>
@@ -25211,7 +25244,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="214" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:20" ht="165" x14ac:dyDescent="0.25">
       <c r="A214" s="13" t="s">
         <v>1374</v>
       </c>
@@ -25262,7 +25295,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="215" spans="1:20" ht="255" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:20" ht="255" x14ac:dyDescent="0.25">
       <c r="A215" s="13" t="s">
         <v>868</v>
       </c>
@@ -25309,7 +25342,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="216" spans="1:20" ht="180" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:20" ht="180" x14ac:dyDescent="0.25">
       <c r="A216" s="13" t="s">
         <v>633</v>
       </c>
@@ -25360,7 +25393,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="217" spans="1:20" ht="225" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:20" ht="225" x14ac:dyDescent="0.25">
       <c r="A217" s="13" t="s">
         <v>679</v>
       </c>
@@ -25411,7 +25444,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="218" spans="1:20" ht="180" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:20" ht="180" x14ac:dyDescent="0.25">
       <c r="A218" s="13" t="s">
         <v>606</v>
       </c>
@@ -25462,7 +25495,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="219" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:20" ht="120" x14ac:dyDescent="0.25">
       <c r="A219" s="13" t="s">
         <v>1913</v>
       </c>
@@ -25513,7 +25546,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="220" spans="1:20" ht="180" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:20" ht="180" x14ac:dyDescent="0.25">
       <c r="A220" s="13" t="s">
         <v>1837</v>
       </c>
@@ -25564,7 +25597,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="221" spans="1:20" ht="255" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:20" ht="255" x14ac:dyDescent="0.25">
       <c r="A221" s="13" t="s">
         <v>1604</v>
       </c>
@@ -25615,7 +25648,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="222" spans="1:20" ht="285" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:20" ht="285" x14ac:dyDescent="0.25">
       <c r="A222" s="13" t="s">
         <v>307</v>
       </c>
@@ -25666,7 +25699,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="223" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:20" ht="105" x14ac:dyDescent="0.25">
       <c r="A223" s="13" t="s">
         <v>1022</v>
       </c>
@@ -25717,7 +25750,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="224" spans="1:20" ht="270" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:20" ht="270" x14ac:dyDescent="0.25">
       <c r="A224" s="13" t="s">
         <v>2064</v>
       </c>
@@ -25768,7 +25801,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="225" spans="1:19" ht="180" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:19" ht="180" x14ac:dyDescent="0.25">
       <c r="A225" s="13" t="s">
         <v>788</v>
       </c>
@@ -25819,7 +25852,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="226" spans="1:19" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:19" ht="135" x14ac:dyDescent="0.25">
       <c r="A226" s="13" t="s">
         <v>1142</v>
       </c>
@@ -25870,7 +25903,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="227" spans="1:19" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:19" ht="90" x14ac:dyDescent="0.25">
       <c r="A227" s="13" t="s">
         <v>1218</v>
       </c>
@@ -25921,7 +25954,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="228" spans="1:19" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:19" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A228" s="13" t="s">
         <v>1617</v>
       </c>
@@ -25968,7 +26001,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="229" spans="1:19" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:19" ht="105" x14ac:dyDescent="0.25">
       <c r="A229" s="13" t="s">
         <v>1171</v>
       </c>
@@ -26019,7 +26052,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="230" spans="1:19" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:19" ht="165" x14ac:dyDescent="0.25">
       <c r="A230" s="13" t="s">
         <v>1844</v>
       </c>
@@ -26070,7 +26103,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="231" spans="1:19" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:19" ht="165" x14ac:dyDescent="0.25">
       <c r="A231" s="13" t="s">
         <v>1149</v>
       </c>
@@ -26475,7 +26508,7 @@
         <v>2902</v>
       </c>
     </row>
-    <row r="238" spans="1:19" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:19" ht="165" x14ac:dyDescent="0.25">
       <c r="A238" s="13" t="s">
         <v>1035</v>
       </c>
@@ -26522,7 +26555,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="239" spans="1:19" ht="180" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:19" ht="180" x14ac:dyDescent="0.25">
       <c r="A239" s="13" t="s">
         <v>315</v>
       </c>
@@ -26573,7 +26606,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="240" spans="1:19" ht="300" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:19" ht="300" x14ac:dyDescent="0.25">
       <c r="A240" s="13" t="s">
         <v>1737</v>
       </c>
@@ -26623,7 +26656,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="241" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:20" ht="120" x14ac:dyDescent="0.25">
       <c r="A241" s="13" t="s">
         <v>2132</v>
       </c>
@@ -26673,7 +26706,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="242" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:20" ht="135" x14ac:dyDescent="0.25">
       <c r="A242" s="13" t="s">
         <v>542</v>
       </c>
@@ -26723,7 +26756,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="243" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:20" ht="135" x14ac:dyDescent="0.25">
       <c r="A243" s="13" t="s">
         <v>639</v>
       </c>
@@ -26773,7 +26806,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="244" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:20" ht="135" x14ac:dyDescent="0.25">
       <c r="A244" s="13" t="s">
         <v>1425</v>
       </c>
@@ -26823,7 +26856,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="245" spans="1:20" ht="255" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:20" ht="255" x14ac:dyDescent="0.25">
       <c r="A245" s="13" t="s">
         <v>795</v>
       </c>
@@ -27039,7 +27072,7 @@
         <v>2368</v>
       </c>
     </row>
-    <row r="249" spans="1:20" ht="195" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:20" ht="195" x14ac:dyDescent="0.25">
       <c r="A249" s="13" t="s">
         <v>816</v>
       </c>
@@ -27093,7 +27126,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="250" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:20" ht="135" x14ac:dyDescent="0.25">
       <c r="A250" s="13" t="s">
         <v>973</v>
       </c>
@@ -27198,7 +27231,7 @@
         <v>2393</v>
       </c>
     </row>
-    <row r="252" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:20" ht="120" x14ac:dyDescent="0.25">
       <c r="A252" s="13" t="s">
         <v>2148</v>
       </c>
@@ -27249,7 +27282,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="253" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:20" ht="165" x14ac:dyDescent="0.25">
       <c r="A253" s="13" t="s">
         <v>1404</v>
       </c>
@@ -27300,7 +27333,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="254" spans="1:20" ht="225" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:20" ht="225" x14ac:dyDescent="0.25">
       <c r="A254" s="13" t="s">
         <v>1111</v>
       </c>
@@ -27351,7 +27384,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="255" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:20" ht="150" x14ac:dyDescent="0.25">
       <c r="A255" s="13" t="s">
         <v>2140</v>
       </c>
@@ -27402,7 +27435,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="256" spans="1:20" ht="360" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:20" ht="360" x14ac:dyDescent="0.25">
       <c r="A256" s="13" t="s">
         <v>1164</v>
       </c>
@@ -27453,7 +27486,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="257" spans="1:20" ht="195" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:20" ht="195" x14ac:dyDescent="0.25">
       <c r="A257" s="13" t="s">
         <v>71</v>
       </c>
@@ -27500,7 +27533,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="258" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:20" ht="165" x14ac:dyDescent="0.25">
       <c r="A258" s="13" t="s">
         <v>1368</v>
       </c>
@@ -27608,7 +27641,7 @@
         <v>2368</v>
       </c>
     </row>
-    <row r="260" spans="1:20" ht="180" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:20" ht="180" x14ac:dyDescent="0.25">
       <c r="A260" s="13" t="s">
         <v>2038</v>
       </c>
@@ -27942,7 +27975,7 @@
         <v>2283</v>
       </c>
     </row>
-    <row r="266" spans="1:20" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:20" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A266" s="13" t="s">
         <v>1934</v>
       </c>
@@ -27993,7 +28026,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="267" spans="1:20" ht="255" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:20" ht="255" x14ac:dyDescent="0.25">
       <c r="A267" s="13" t="s">
         <v>1042</v>
       </c>
@@ -28044,7 +28077,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="268" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:20" ht="165" x14ac:dyDescent="0.25">
       <c r="A268" s="13" t="s">
         <v>2072</v>
       </c>
@@ -28219,7 +28252,7 @@
         <v>2369</v>
       </c>
     </row>
-    <row r="271" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:20" ht="120" x14ac:dyDescent="0.25">
       <c r="A271" s="13" t="s">
         <v>1817</v>
       </c>
@@ -28270,7 +28303,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="272" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:20" ht="120" x14ac:dyDescent="0.25">
       <c r="A272" s="13" t="s">
         <v>1684</v>
       </c>
@@ -28321,7 +28354,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="273" spans="1:19" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:19" ht="120" x14ac:dyDescent="0.25">
       <c r="A273" s="13" t="s">
         <v>1076</v>
       </c>
@@ -28422,7 +28455,7 @@
         <v>2873</v>
       </c>
     </row>
-    <row r="275" spans="1:19" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:19" ht="150" x14ac:dyDescent="0.25">
       <c r="A275" s="13" t="s">
         <v>1506</v>
       </c>
@@ -28473,7 +28506,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="276" spans="1:19" ht="270" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:19" ht="270" x14ac:dyDescent="0.25">
       <c r="A276" s="13" t="s">
         <v>765</v>
       </c>
@@ -28520,7 +28553,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="277" spans="1:19" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:19" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A277" s="13" t="s">
         <v>1329</v>
       </c>
@@ -28574,7 +28607,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="278" spans="1:19" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:19" ht="165" x14ac:dyDescent="0.25">
       <c r="A278" s="13" t="s">
         <v>223</v>
       </c>
@@ -28625,7 +28658,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="279" spans="1:19" ht="225" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:19" ht="225" x14ac:dyDescent="0.25">
       <c r="A279" s="13" t="s">
         <v>2006</v>
       </c>
@@ -28672,7 +28705,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="280" spans="1:19" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:19" ht="165" x14ac:dyDescent="0.25">
       <c r="A280" s="13" t="s">
         <v>901</v>
       </c>
@@ -28723,7 +28756,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="281" spans="1:19" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:19" ht="165" x14ac:dyDescent="0.25">
       <c r="A281" s="13" t="s">
         <v>360</v>
       </c>
@@ -28774,7 +28807,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="282" spans="1:19" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:19" ht="150" x14ac:dyDescent="0.25">
       <c r="A282" s="13" t="s">
         <v>1465</v>
       </c>
@@ -28825,7 +28858,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="283" spans="1:19" ht="195" hidden="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:19" ht="195" x14ac:dyDescent="0.25">
       <c r="A283" s="13" t="s">
         <v>1710</v>
       </c>
@@ -28876,7 +28909,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="284" spans="1:19" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:19" ht="165" x14ac:dyDescent="0.25">
       <c r="A284" s="13" t="s">
         <v>1204</v>
       </c>
@@ -28927,7 +28960,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="285" spans="1:19" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:19" ht="165" x14ac:dyDescent="0.25">
       <c r="A285" s="13" t="s">
         <v>108</v>
       </c>
@@ -28974,7 +29007,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="286" spans="1:19" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:19" ht="105" x14ac:dyDescent="0.25">
       <c r="A286" s="13" t="s">
         <v>2099</v>
       </c>
@@ -29025,7 +29058,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="287" spans="1:19" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:19" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A287" s="13" t="s">
         <v>881</v>
       </c>
@@ -29072,7 +29105,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="288" spans="1:19" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:19" ht="120" x14ac:dyDescent="0.25">
       <c r="A288" s="13" t="s">
         <v>1698</v>
       </c>
@@ -29123,7 +29156,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="289" spans="1:19" ht="195" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:19" ht="195" x14ac:dyDescent="0.25">
       <c r="A289" s="13" t="s">
         <v>1804</v>
       </c>
@@ -29174,7 +29207,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="290" spans="1:19" ht="210" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:19" ht="210" x14ac:dyDescent="0.25">
       <c r="A290" s="13" t="s">
         <v>1059</v>
       </c>
@@ -29281,7 +29314,7 @@
         <v>2179</v>
       </c>
     </row>
-    <row r="292" spans="1:19" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:19" ht="105" x14ac:dyDescent="0.25">
       <c r="A292" s="13" t="s">
         <v>1598</v>
       </c>
@@ -29331,7 +29364,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="293" spans="1:19" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:19" ht="150" x14ac:dyDescent="0.25">
       <c r="A293" s="13" t="s">
         <v>808</v>
       </c>
@@ -29385,7 +29418,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="294" spans="1:19" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:19" ht="150" x14ac:dyDescent="0.25">
       <c r="A294" s="13" t="s">
         <v>1361</v>
       </c>
@@ -29439,7 +29472,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="295" spans="1:19" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:19" ht="150" x14ac:dyDescent="0.25">
       <c r="A295" s="13" t="s">
         <v>1656</v>
       </c>
@@ -29493,7 +29526,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="296" spans="1:19" ht="195" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:19" ht="195" x14ac:dyDescent="0.25">
       <c r="A296" s="13" t="s">
         <v>719</v>
       </c>
@@ -29547,7 +29580,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="297" spans="1:19" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:19" ht="165" x14ac:dyDescent="0.25">
       <c r="A297" s="13" t="s">
         <v>1103</v>
       </c>
@@ -29601,7 +29634,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="298" spans="1:19" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:19" ht="150" x14ac:dyDescent="0.25">
       <c r="A298" s="13" t="s">
         <v>233</v>
       </c>
@@ -29655,7 +29688,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="299" spans="1:19" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:19" ht="165" x14ac:dyDescent="0.25">
       <c r="A299" s="13" t="s">
         <v>613</v>
       </c>
@@ -29709,7 +29742,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="300" spans="1:19" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:19" ht="165" x14ac:dyDescent="0.25">
       <c r="A300" s="13" t="s">
         <v>826</v>
       </c>
@@ -29763,7 +29796,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="301" spans="1:19" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:19" ht="135" x14ac:dyDescent="0.25">
       <c r="A301" s="13" t="s">
         <v>1950</v>
       </c>
@@ -29917,7 +29950,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="304" spans="1:19" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:19" ht="90" x14ac:dyDescent="0.25">
       <c r="A304" s="13" t="s">
         <v>1885</v>
       </c>
@@ -29969,11 +30002,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U304">
-    <filterColumn colId="0">
-      <colorFilter dxfId="0"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:U304"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>